<commit_message>
junit Test fuer Transformation eingebaut, Maven Build wirft einen Fehler bei junit.assert.fail, der in Eclipse nicht auftritt
</commit_message>
<xml_diff>
--- a/cda_basismodul/Basismodul V2015.1-VT.xlsx
+++ b/cda_basismodul/Basismodul V2015.1-VT.xlsx
@@ -7483,27 +7483,28 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -7514,16 +7515,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18132,8 +18132,8 @@
   </sheetPr>
   <dimension ref="A1:Y564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210"/>
+    <sheetView tabSelected="1" topLeftCell="A353" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F366" sqref="F366:F367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18163,41 +18163,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="138" t="s">
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="139" t="s">
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="140" t="s">
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
+      <c r="T1" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="140"/>
-      <c r="V1" s="140"/>
-      <c r="W1" s="140"/>
-      <c r="X1" s="141" t="s">
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="141"/>
+      <c r="Y1" s="134"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -18300,7 +18300,7 @@
         <f>IF(G3&lt;&gt;"",VLOOKUP(G3,'DE-EN'!$A$2:$B$799,2,FALSE),"")</f>
         <v>ID</v>
       </c>
-      <c r="I3" s="134" t="s">
+      <c r="I3" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J3" s="88">
@@ -18325,7 +18325,7 @@
         <v>5</v>
       </c>
       <c r="S3" s="88"/>
-      <c r="T3" s="129" t="s">
+      <c r="T3" s="130" t="s">
         <v>547</v>
       </c>
       <c r="U3" s="55"/>
@@ -18352,7 +18352,7 @@
         <f>IF(G4&lt;&gt;"",VLOOKUP(G4,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>hospital</v>
       </c>
-      <c r="I4" s="134"/>
+      <c r="I4" s="128"/>
       <c r="J4" s="88">
         <v>22232009</v>
       </c>
@@ -18373,7 +18373,7 @@
       </c>
       <c r="R4" s="88"/>
       <c r="S4" s="88"/>
-      <c r="T4" s="129"/>
+      <c r="T4" s="130"/>
       <c r="U4" s="55"/>
       <c r="V4" s="93"/>
       <c r="W4" s="55"/>
@@ -18403,7 +18403,7 @@
         <f>IF(G5&lt;&gt;"",VLOOKUP(G5,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>ID</v>
       </c>
-      <c r="I5" s="133" t="s">
+      <c r="I5" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J5" s="89">
@@ -18430,7 +18430,7 @@
       <c r="R5" s="65">
         <v>3</v>
       </c>
-      <c r="T5" s="130" t="s">
+      <c r="T5" s="135" t="s">
         <v>547</v>
       </c>
       <c r="X5" s="8" t="s">
@@ -18448,7 +18448,7 @@
         <f>IF(G6&lt;&gt;"",VLOOKUP(G6,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>emergency department</v>
       </c>
-      <c r="I6" s="133"/>
+      <c r="I6" s="129"/>
       <c r="J6" s="89">
         <v>225728007</v>
       </c>
@@ -18461,7 +18461,7 @@
       <c r="M6" s="89">
         <v>3</v>
       </c>
-      <c r="T6" s="130"/>
+      <c r="T6" s="135"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="G7" s="89" t="s">
@@ -18532,7 +18532,7 @@
       </c>
       <c r="R8" s="103"/>
       <c r="S8" s="88"/>
-      <c r="T8" s="129" t="s">
+      <c r="T8" s="130" t="s">
         <v>548</v>
       </c>
       <c r="U8" s="55"/>
@@ -18578,7 +18578,7 @@
       <c r="Q9" s="88"/>
       <c r="R9" s="88"/>
       <c r="S9" s="88"/>
-      <c r="T9" s="129"/>
+      <c r="T9" s="130"/>
       <c r="U9" s="55"/>
       <c r="V9" s="93"/>
       <c r="W9" s="55"/>
@@ -18816,19 +18816,19 @@
         <v xml:space="preserve">insurance  </v>
       </c>
       <c r="I17" s="93"/>
-      <c r="J17" s="129">
+      <c r="J17" s="130">
         <v>398174006</v>
       </c>
-      <c r="K17" s="129" t="s">
+      <c r="K17" s="130" t="s">
         <v>676</v>
       </c>
-      <c r="L17" s="129" t="s">
+      <c r="L17" s="130" t="s">
         <v>370</v>
       </c>
-      <c r="M17" s="129">
+      <c r="M17" s="130">
         <v>5</v>
       </c>
-      <c r="N17" s="129" t="s">
+      <c r="N17" s="130" t="s">
         <v>759</v>
       </c>
       <c r="O17" s="88" t="s">
@@ -18870,11 +18870,11 @@
         <v>name</v>
       </c>
       <c r="I18" s="93"/>
-      <c r="J18" s="129"/>
-      <c r="K18" s="129"/>
-      <c r="L18" s="129"/>
-      <c r="M18" s="129"/>
-      <c r="N18" s="129"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="130"/>
+      <c r="L18" s="130"/>
+      <c r="M18" s="130"/>
+      <c r="N18" s="130"/>
       <c r="O18" s="88"/>
       <c r="P18" s="88"/>
       <c r="Q18" s="88"/>
@@ -18910,37 +18910,37 @@
         <f>IF(G19&lt;&gt;"",VLOOKUP(G19,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient</v>
       </c>
-      <c r="J19" s="130">
+      <c r="J19" s="135">
         <v>371484003</v>
       </c>
-      <c r="K19" s="130" t="s">
+      <c r="K19" s="135" t="s">
         <v>677</v>
       </c>
-      <c r="L19" s="130" t="s">
+      <c r="L19" s="135" t="s">
         <v>370</v>
       </c>
-      <c r="M19" s="130">
+      <c r="M19" s="135">
         <v>1</v>
       </c>
-      <c r="O19" s="130" t="s">
+      <c r="O19" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P19" s="130" t="s">
+      <c r="P19" s="135" t="s">
         <v>614</v>
       </c>
-      <c r="Q19" s="130" t="s">
+      <c r="Q19" s="135" t="s">
         <v>615</v>
       </c>
-      <c r="R19" s="130">
+      <c r="R19" s="135">
         <v>1</v>
       </c>
-      <c r="T19" s="130" t="s">
+      <c r="T19" s="135" t="s">
         <v>2025</v>
       </c>
-      <c r="U19" s="130" t="s">
+      <c r="U19" s="135" t="s">
         <v>549</v>
       </c>
-      <c r="V19" s="133" t="s">
+      <c r="V19" s="129" t="s">
         <v>339</v>
       </c>
       <c r="W19" s="89"/>
@@ -18959,17 +18959,17 @@
         <f>IF(G20&lt;&gt;"",VLOOKUP(G20,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>name</v>
       </c>
-      <c r="J20" s="130"/>
-      <c r="K20" s="130"/>
-      <c r="L20" s="130"/>
-      <c r="M20" s="130"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="130"/>
-      <c r="Q20" s="130"/>
-      <c r="R20" s="130"/>
-      <c r="T20" s="130"/>
-      <c r="U20" s="130"/>
-      <c r="V20" s="133"/>
+      <c r="J20" s="135"/>
+      <c r="K20" s="135"/>
+      <c r="L20" s="135"/>
+      <c r="M20" s="135"/>
+      <c r="O20" s="135"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="135"/>
+      <c r="R20" s="135"/>
+      <c r="T20" s="135"/>
+      <c r="U20" s="135"/>
+      <c r="V20" s="129"/>
       <c r="W20" s="89"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -18996,7 +18996,7 @@
         <f>IF(G21&lt;&gt;"",VLOOKUP(G21,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient address</v>
       </c>
-      <c r="I21" s="134" t="s">
+      <c r="I21" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J21" s="88">
@@ -19056,7 +19056,7 @@
         <f>IF(G22&lt;&gt;"",VLOOKUP(G22,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>street</v>
       </c>
-      <c r="I22" s="134"/>
+      <c r="I22" s="128"/>
       <c r="J22" s="88">
         <v>398099009</v>
       </c>
@@ -19253,7 +19253,7 @@
         <f>IF(G26&lt;&gt;"",VLOOKUP(G26,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient address</v>
       </c>
-      <c r="I26" s="134" t="s">
+      <c r="I26" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J26" s="88">
@@ -19312,7 +19312,7 @@
       <c r="H27" s="94" t="s">
         <v>1950</v>
       </c>
-      <c r="I27" s="134"/>
+      <c r="I27" s="128"/>
       <c r="J27" s="88">
         <v>433178008</v>
       </c>
@@ -19365,7 +19365,7 @@
         <f>IF(G28&lt;&gt;"",VLOOKUP(G28,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient address</v>
       </c>
-      <c r="I28" s="133" t="s">
+      <c r="I28" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J28" s="89">
@@ -19416,7 +19416,7 @@
         <f>IF(G29&lt;&gt;"",VLOOKUP(G29,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>telephone number</v>
       </c>
-      <c r="I29" s="133"/>
+      <c r="I29" s="129"/>
       <c r="J29" s="89">
         <v>184103008</v>
       </c>
@@ -19468,16 +19468,16 @@
         <v>1487</v>
       </c>
       <c r="I30" s="93"/>
-      <c r="J30" s="129">
+      <c r="J30" s="130">
         <v>184099003</v>
       </c>
-      <c r="K30" s="129" t="s">
+      <c r="K30" s="130" t="s">
         <v>683</v>
       </c>
-      <c r="L30" s="129" t="s">
+      <c r="L30" s="130" t="s">
         <v>370</v>
       </c>
-      <c r="M30" s="129" t="s">
+      <c r="M30" s="130" t="s">
         <v>684</v>
       </c>
       <c r="N30" s="88"/>
@@ -19525,10 +19525,10 @@
         <v>674</v>
       </c>
       <c r="I31" s="93"/>
-      <c r="J31" s="129"/>
-      <c r="K31" s="129"/>
-      <c r="L31" s="129"/>
-      <c r="M31" s="129"/>
+      <c r="J31" s="130"/>
+      <c r="K31" s="130"/>
+      <c r="L31" s="130"/>
+      <c r="M31" s="130"/>
       <c r="N31" s="88"/>
       <c r="O31" s="88"/>
       <c r="P31" s="88"/>
@@ -19562,7 +19562,7 @@
         <f>IF(G32&lt;&gt;"",VLOOKUP(G32,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin Scale Score</v>
       </c>
-      <c r="I32" s="133" t="s">
+      <c r="I32" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J32" s="89">
@@ -19610,7 +19610,7 @@
         <f>IF(G33&lt;&gt;"",VLOOKUP(G33,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 0</v>
       </c>
-      <c r="I33" s="133"/>
+      <c r="I33" s="129"/>
       <c r="J33" s="89">
         <v>276727009</v>
       </c>
@@ -19647,7 +19647,7 @@
         <f>IF(G34&lt;&gt;"",VLOOKUP(G34,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 1</v>
       </c>
-      <c r="I34" s="133"/>
+      <c r="I34" s="129"/>
       <c r="J34" s="89">
         <v>38112003</v>
       </c>
@@ -19684,7 +19684,7 @@
         <f>IF(G35&lt;&gt;"",VLOOKUP(G35,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 2</v>
       </c>
-      <c r="I35" s="133"/>
+      <c r="I35" s="129"/>
       <c r="J35" s="89">
         <v>19338005</v>
       </c>
@@ -19718,7 +19718,7 @@
         <f>IF(G36&lt;&gt;"",VLOOKUP(G36,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 3</v>
       </c>
-      <c r="I36" s="133"/>
+      <c r="I36" s="129"/>
       <c r="J36" s="89">
         <v>79605009</v>
       </c>
@@ -19752,7 +19752,7 @@
         <f>IF(G37&lt;&gt;"",VLOOKUP(G37,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 4</v>
       </c>
-      <c r="I37" s="133"/>
+      <c r="I37" s="129"/>
       <c r="J37" s="89">
         <v>9362000</v>
       </c>
@@ -19786,7 +19786,7 @@
         <f>IF(G38&lt;&gt;"",VLOOKUP(G38,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 5</v>
       </c>
-      <c r="I38" s="133"/>
+      <c r="I38" s="129"/>
       <c r="J38" s="89">
         <v>34001005</v>
       </c>
@@ -19820,7 +19820,7 @@
         <f>IF(G39&lt;&gt;"",VLOOKUP(G39,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Rankin 6</v>
       </c>
-      <c r="I39" s="133"/>
+      <c r="I39" s="129"/>
       <c r="J39" s="89">
         <v>68244004</v>
       </c>
@@ -20072,28 +20072,28 @@
         <f>IF(G44&lt;&gt;"",VLOOKUP(G44,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>admission</v>
       </c>
-      <c r="J44" s="130">
+      <c r="J44" s="135">
         <v>399423000</v>
       </c>
-      <c r="K44" s="130" t="s">
+      <c r="K44" s="135" t="s">
         <v>695</v>
       </c>
-      <c r="L44" s="130" t="s">
+      <c r="L44" s="135" t="s">
         <v>370</v>
       </c>
-      <c r="M44" s="130">
+      <c r="M44" s="135">
         <v>1</v>
       </c>
-      <c r="O44" s="130" t="s">
+      <c r="O44" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P44" s="130" t="s">
+      <c r="P44" s="135" t="s">
         <v>604</v>
       </c>
-      <c r="Q44" s="130" t="s">
+      <c r="Q44" s="135" t="s">
         <v>605</v>
       </c>
-      <c r="R44" s="130">
+      <c r="R44" s="135">
         <v>1</v>
       </c>
       <c r="T44" s="89" t="s">
@@ -20120,14 +20120,14 @@
         <f>IF(G45&lt;&gt;"",VLOOKUP(G45,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>date</v>
       </c>
-      <c r="J45" s="130"/>
-      <c r="K45" s="130"/>
-      <c r="L45" s="130"/>
-      <c r="M45" s="130"/>
-      <c r="O45" s="130"/>
-      <c r="P45" s="130"/>
-      <c r="Q45" s="130"/>
-      <c r="R45" s="130"/>
+      <c r="J45" s="135"/>
+      <c r="K45" s="135"/>
+      <c r="L45" s="135"/>
+      <c r="M45" s="135"/>
+      <c r="O45" s="135"/>
+      <c r="P45" s="135"/>
+      <c r="Q45" s="135"/>
+      <c r="R45" s="135"/>
       <c r="V45" s="36"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
@@ -20154,7 +20154,7 @@
         <f>IF(G46&lt;&gt;"",VLOOKUP(G46,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>admission</v>
       </c>
-      <c r="I46" s="134" t="s">
+      <c r="I46" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J46" s="88">
@@ -20216,7 +20216,7 @@
         <f>IF(G47&lt;&gt;"",VLOOKUP(G47,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>time</v>
       </c>
-      <c r="I47" s="134"/>
+      <c r="I47" s="128"/>
       <c r="J47" s="88">
         <v>410670007</v>
       </c>
@@ -20445,7 +20445,7 @@
         <f>IF(G53&lt;&gt;"",VLOOKUP(G53,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>tetanus status</v>
       </c>
-      <c r="I53" s="134" t="s">
+      <c r="I53" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J53" s="88">
@@ -20501,7 +20501,7 @@
         <f>IF(G54&lt;&gt;"",VLOOKUP(G54,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient</v>
       </c>
-      <c r="I54" s="134"/>
+      <c r="I54" s="128"/>
       <c r="J54" s="88">
         <v>116154003</v>
       </c>
@@ -20543,7 +20543,7 @@
         <f>IF(G55&lt;&gt;"",VLOOKUP(G55,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>active tetanus vaccination</v>
       </c>
-      <c r="I55" s="134"/>
+      <c r="I55" s="128"/>
       <c r="J55" s="88">
         <v>52101004</v>
       </c>
@@ -20585,7 +20585,7 @@
         <f>IF(G56&lt;&gt;"",VLOOKUP(G56,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>no tetanus vaccination</v>
       </c>
-      <c r="I56" s="134"/>
+      <c r="I56" s="128"/>
       <c r="J56" s="88">
         <v>41277001</v>
       </c>
@@ -20627,7 +20627,7 @@
         <f>IF(G57&lt;&gt;"",VLOOKUP(G57,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>information not leviable</v>
       </c>
-      <c r="I57" s="134"/>
+      <c r="I57" s="128"/>
       <c r="J57" s="88">
         <v>103314005</v>
       </c>
@@ -20678,7 +20678,7 @@
       <c r="H58" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="I58" s="133" t="s">
+      <c r="I58" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J58" s="91">
@@ -20726,7 +20726,7 @@
         <f>IF(G59&lt;&gt;"",VLOOKUP(G59,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient</v>
       </c>
-      <c r="I59" s="133"/>
+      <c r="I59" s="129"/>
       <c r="J59" s="75">
         <v>116154003</v>
       </c>
@@ -20757,7 +20757,7 @@
         <f>IF(G60&lt;&gt;"",VLOOKUP(G60,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Isolation necessary</v>
       </c>
-      <c r="I60" s="133"/>
+      <c r="I60" s="129"/>
       <c r="J60" s="91">
         <v>410525008</v>
       </c>
@@ -20788,7 +20788,7 @@
         <f>IF(G61&lt;&gt;"",VLOOKUP(G61,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Isolation not necessary</v>
       </c>
-      <c r="I61" s="133"/>
+      <c r="I61" s="129"/>
       <c r="J61" s="89">
         <v>410529002</v>
       </c>
@@ -20832,7 +20832,7 @@
         <f>IF(G62&lt;&gt;"",VLOOKUP(G62,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>isolation</v>
       </c>
-      <c r="I62" s="134" t="s">
+      <c r="I62" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J62" s="88">
@@ -20888,7 +20888,7 @@
         <f>IF(G63&lt;&gt;"",VLOOKUP(G63,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>reason</v>
       </c>
-      <c r="I63" s="134"/>
+      <c r="I63" s="128"/>
       <c r="J63" s="88">
         <v>410666004</v>
       </c>
@@ -22059,7 +22059,7 @@
         <f>IF(G94&lt;&gt;"",VLOOKUP(G94,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>GCS verbal answer</v>
       </c>
-      <c r="I94" s="134" t="s">
+      <c r="I94" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J94" s="88">
@@ -22115,7 +22115,7 @@
         <f>IF(G95&lt;&gt;"",VLOOKUP(G95,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>inital</v>
       </c>
-      <c r="I95" s="134"/>
+      <c r="I95" s="128"/>
       <c r="J95" s="88">
         <v>884001</v>
       </c>
@@ -22157,7 +22157,7 @@
         <f>IF(G96&lt;&gt;"",VLOOKUP(G96,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>none</v>
       </c>
-      <c r="I96" s="134"/>
+      <c r="I96" s="128"/>
       <c r="J96" s="88">
         <v>373067005</v>
       </c>
@@ -22205,7 +22205,7 @@
         <f>IF(G97&lt;&gt;"",VLOOKUP(G97,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>verbal</v>
       </c>
-      <c r="I97" s="134"/>
+      <c r="I97" s="128"/>
       <c r="J97" s="88">
         <v>255373000</v>
       </c>
@@ -22245,7 +22245,7 @@
         <f>IF(G98&lt;&gt;"",VLOOKUP(G98,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>response</v>
       </c>
-      <c r="I98" s="134"/>
+      <c r="I98" s="128"/>
       <c r="J98" s="88">
         <v>248237001</v>
       </c>
@@ -22287,7 +22287,7 @@
         <f>IF(G99&lt;&gt;"",VLOOKUP(G99,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>incomprehensible</v>
       </c>
-      <c r="I99" s="134"/>
+      <c r="I99" s="128"/>
       <c r="J99" s="88">
         <v>53314000</v>
       </c>
@@ -22335,7 +22335,7 @@
         <f>IF(G100&lt;&gt;"",VLOOKUP(G100,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>verbal</v>
       </c>
-      <c r="I100" s="134"/>
+      <c r="I100" s="128"/>
       <c r="J100" s="88">
         <v>255373000</v>
       </c>
@@ -22375,7 +22375,7 @@
         <f>IF(G101&lt;&gt;"",VLOOKUP(G101,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>response</v>
       </c>
-      <c r="I101" s="134"/>
+      <c r="I101" s="128"/>
       <c r="J101" s="88">
         <v>248237001</v>
       </c>
@@ -22417,7 +22417,7 @@
         <f>IF(G102&lt;&gt;"",VLOOKUP(G102,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>inadequate</v>
       </c>
-      <c r="I102" s="134"/>
+      <c r="I102" s="128"/>
       <c r="J102" s="88">
         <v>71978007</v>
       </c>
@@ -22465,7 +22465,7 @@
         <f>IF(G103&lt;&gt;"",VLOOKUP(G103,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>verbal</v>
       </c>
-      <c r="I103" s="134"/>
+      <c r="I103" s="128"/>
       <c r="J103" s="88">
         <v>255373000</v>
       </c>
@@ -22505,7 +22505,7 @@
         <f>IF(G104&lt;&gt;"",VLOOKUP(G104,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>response</v>
       </c>
-      <c r="I104" s="134"/>
+      <c r="I104" s="128"/>
       <c r="J104" s="88">
         <v>248237001</v>
       </c>
@@ -22547,7 +22547,7 @@
         <f>IF(G105&lt;&gt;"",VLOOKUP(G105,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>confused</v>
       </c>
-      <c r="I105" s="134"/>
+      <c r="I105" s="128"/>
       <c r="J105" s="88">
         <v>40917007</v>
       </c>
@@ -22595,7 +22595,7 @@
         <f>IF(G106&lt;&gt;"",VLOOKUP(G106,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>verbal</v>
       </c>
-      <c r="I106" s="134"/>
+      <c r="I106" s="128"/>
       <c r="J106" s="88">
         <v>255373000</v>
       </c>
@@ -22635,7 +22635,7 @@
         <f>IF(G107&lt;&gt;"",VLOOKUP(G107,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>response</v>
       </c>
-      <c r="I107" s="134"/>
+      <c r="I107" s="128"/>
       <c r="J107" s="88">
         <v>248237001</v>
       </c>
@@ -22677,7 +22677,7 @@
         <f>IF(G108&lt;&gt;"",VLOOKUP(G108,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>oriented</v>
       </c>
-      <c r="I108" s="134"/>
+      <c r="I108" s="128"/>
       <c r="J108" s="88">
         <v>247663003</v>
       </c>
@@ -22725,7 +22725,7 @@
         <f>IF(G109&lt;&gt;"",VLOOKUP(G109,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>verbal</v>
       </c>
-      <c r="I109" s="134"/>
+      <c r="I109" s="128"/>
       <c r="J109" s="88">
         <v>255373000</v>
       </c>
@@ -22765,7 +22765,7 @@
         <f>IF(G110&lt;&gt;"",VLOOKUP(G110,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>response</v>
       </c>
-      <c r="I110" s="134"/>
+      <c r="I110" s="128"/>
       <c r="J110" s="88">
         <v>248237001</v>
       </c>
@@ -22811,7 +22811,7 @@
         <f>IF(G111&lt;&gt;"",VLOOKUP(G111,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>GCS motor response</v>
       </c>
-      <c r="I111" s="133" t="s">
+      <c r="I111" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J111" s="89">
@@ -22856,7 +22856,7 @@
         <f>IF(G112&lt;&gt;"",VLOOKUP(G112,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>inital</v>
       </c>
-      <c r="I112" s="133"/>
+      <c r="I112" s="129"/>
       <c r="J112" s="89">
         <v>884001</v>
       </c>
@@ -22875,14 +22875,14 @@
       <c r="F113" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G113" s="130" t="s">
+      <c r="G113" s="135" t="s">
         <v>143</v>
       </c>
-      <c r="H113" s="136" t="str">
+      <c r="H113" s="140" t="str">
         <f>IF(G113&lt;&gt;"",VLOOKUP(G113,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>none</v>
       </c>
-      <c r="I113" s="133"/>
+      <c r="I113" s="129"/>
       <c r="J113" s="89">
         <v>373067005</v>
       </c>
@@ -22895,13 +22895,13 @@
       <c r="M113" s="89">
         <v>2</v>
       </c>
-      <c r="O113" s="131" t="s">
+      <c r="O113" s="139" t="s">
         <v>388</v>
       </c>
-      <c r="P113" s="130" t="s">
+      <c r="P113" s="135" t="s">
         <v>2059</v>
       </c>
-      <c r="Q113" s="130" t="s">
+      <c r="Q113" s="135" t="s">
         <v>592</v>
       </c>
       <c r="R113" s="89">
@@ -22909,9 +22909,9 @@
       </c>
     </row>
     <row r="114" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G114" s="130"/>
-      <c r="H114" s="136"/>
-      <c r="I114" s="133"/>
+      <c r="G114" s="135"/>
+      <c r="H114" s="140"/>
+      <c r="I114" s="129"/>
       <c r="J114" s="89">
         <v>255324009</v>
       </c>
@@ -22924,14 +22924,14 @@
       <c r="M114" s="89">
         <v>4</v>
       </c>
-      <c r="O114" s="131"/>
-      <c r="P114" s="130"/>
-      <c r="Q114" s="130"/>
+      <c r="O114" s="139"/>
+      <c r="P114" s="135"/>
+      <c r="Q114" s="135"/>
     </row>
     <row r="115" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G115" s="130"/>
-      <c r="H115" s="136"/>
-      <c r="I115" s="133"/>
+      <c r="G115" s="135"/>
+      <c r="H115" s="140"/>
+      <c r="I115" s="129"/>
       <c r="J115" s="89">
         <v>248237001</v>
       </c>
@@ -22944,22 +22944,22 @@
       <c r="M115" s="89">
         <v>3</v>
       </c>
-      <c r="O115" s="131"/>
-      <c r="P115" s="130"/>
-      <c r="Q115" s="130"/>
+      <c r="O115" s="139"/>
+      <c r="P115" s="135"/>
+      <c r="Q115" s="135"/>
     </row>
     <row r="116" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F116" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G116" s="130" t="s">
+      <c r="G116" s="135" t="s">
         <v>167</v>
       </c>
-      <c r="H116" s="136" t="str">
+      <c r="H116" s="140" t="str">
         <f>IF(G116&lt;&gt;"",VLOOKUP(G116,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>stretching movement</v>
       </c>
-      <c r="I116" s="133"/>
+      <c r="I116" s="129"/>
       <c r="J116" s="89">
         <v>129420008</v>
       </c>
@@ -22972,13 +22972,13 @@
       <c r="M116" s="89">
         <v>2</v>
       </c>
-      <c r="O116" s="130" t="s">
+      <c r="O116" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P116" s="130" t="s">
+      <c r="P116" s="135" t="s">
         <v>2060</v>
       </c>
-      <c r="Q116" s="130" t="s">
+      <c r="Q116" s="135" t="s">
         <v>593</v>
       </c>
       <c r="R116" s="89">
@@ -22986,9 +22986,9 @@
       </c>
     </row>
     <row r="117" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G117" s="130"/>
-      <c r="H117" s="136"/>
-      <c r="I117" s="133"/>
+      <c r="G117" s="135"/>
+      <c r="H117" s="140"/>
+      <c r="I117" s="129"/>
       <c r="J117" s="89">
         <v>255324009</v>
       </c>
@@ -23001,9 +23001,9 @@
       <c r="M117" s="89">
         <v>2</v>
       </c>
-      <c r="O117" s="130"/>
-      <c r="P117" s="130"/>
-      <c r="Q117" s="130"/>
+      <c r="O117" s="135"/>
+      <c r="P117" s="135"/>
+      <c r="Q117" s="135"/>
     </row>
     <row r="118" spans="6:18" x14ac:dyDescent="0.25">
       <c r="G118" s="89" t="s">
@@ -23013,7 +23013,7 @@
         <f>IF(G118&lt;&gt;"",VLOOKUP(G118,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>to stimuli</v>
       </c>
-      <c r="I118" s="133"/>
+      <c r="I118" s="129"/>
       <c r="J118" s="89">
         <v>248237001</v>
       </c>
@@ -23026,22 +23026,22 @@
       <c r="M118" s="89">
         <v>3</v>
       </c>
-      <c r="O118" s="130"/>
-      <c r="P118" s="130"/>
-      <c r="Q118" s="130"/>
+      <c r="O118" s="135"/>
+      <c r="P118" s="135"/>
+      <c r="Q118" s="135"/>
     </row>
     <row r="119" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F119" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="G119" s="130" t="s">
+      <c r="G119" s="135" t="s">
         <v>766</v>
       </c>
-      <c r="H119" s="136" t="str">
+      <c r="H119" s="140" t="str">
         <f>IF(G119&lt;&gt;"",VLOOKUP(G119,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>bend movement</v>
       </c>
-      <c r="I119" s="133"/>
+      <c r="I119" s="129"/>
       <c r="J119" s="89">
         <v>282977007</v>
       </c>
@@ -23054,13 +23054,13 @@
       <c r="M119" s="89">
         <v>2</v>
       </c>
-      <c r="O119" s="130" t="s">
+      <c r="O119" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P119" s="130" t="s">
+      <c r="P119" s="135" t="s">
         <v>2061</v>
       </c>
-      <c r="Q119" s="130" t="s">
+      <c r="Q119" s="135" t="s">
         <v>594</v>
       </c>
       <c r="R119" s="89">
@@ -23068,9 +23068,9 @@
       </c>
     </row>
     <row r="120" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G120" s="130"/>
-      <c r="H120" s="136"/>
-      <c r="I120" s="133"/>
+      <c r="G120" s="135"/>
+      <c r="H120" s="140"/>
+      <c r="I120" s="129"/>
       <c r="J120" s="89">
         <v>255324009</v>
       </c>
@@ -23083,9 +23083,9 @@
       <c r="M120" s="89">
         <v>1</v>
       </c>
-      <c r="O120" s="130"/>
-      <c r="P120" s="130"/>
-      <c r="Q120" s="130"/>
+      <c r="O120" s="135"/>
+      <c r="P120" s="135"/>
+      <c r="Q120" s="135"/>
     </row>
     <row r="121" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G121" s="89" t="s">
@@ -23095,7 +23095,7 @@
         <f>IF(G121&lt;&gt;"",VLOOKUP(G121,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>to stimuli</v>
       </c>
-      <c r="I121" s="133"/>
+      <c r="I121" s="129"/>
       <c r="J121" s="89">
         <v>248237001</v>
       </c>
@@ -23108,22 +23108,22 @@
       <c r="M121" s="89">
         <v>3</v>
       </c>
-      <c r="O121" s="130"/>
-      <c r="P121" s="130"/>
-      <c r="Q121" s="130"/>
+      <c r="O121" s="135"/>
+      <c r="P121" s="135"/>
+      <c r="Q121" s="135"/>
     </row>
     <row r="122" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F122" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G122" s="130" t="s">
+      <c r="G122" s="135" t="s">
         <v>171</v>
       </c>
-      <c r="H122" s="136" t="str">
+      <c r="H122" s="140" t="str">
         <f>IF(G122&lt;&gt;"",VLOOKUP(G122,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>untargeted movement</v>
       </c>
-      <c r="I122" s="133"/>
+      <c r="I122" s="129"/>
       <c r="J122" s="89">
         <v>62476001</v>
       </c>
@@ -23136,13 +23136,13 @@
       <c r="M122" s="89">
         <v>2</v>
       </c>
-      <c r="O122" s="130" t="s">
+      <c r="O122" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P122" s="130" t="s">
+      <c r="P122" s="135" t="s">
         <v>2062</v>
       </c>
-      <c r="Q122" s="130" t="s">
+      <c r="Q122" s="135" t="s">
         <v>595</v>
       </c>
       <c r="R122" s="89">
@@ -23150,9 +23150,9 @@
       </c>
     </row>
     <row r="123" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G123" s="130"/>
-      <c r="H123" s="136"/>
-      <c r="I123" s="133"/>
+      <c r="G123" s="135"/>
+      <c r="H123" s="140"/>
+      <c r="I123" s="129"/>
       <c r="J123" s="89">
         <v>255324009</v>
       </c>
@@ -23165,18 +23165,18 @@
       <c r="M123" s="89">
         <v>1</v>
       </c>
-      <c r="O123" s="130"/>
-      <c r="P123" s="130"/>
-      <c r="Q123" s="130"/>
+      <c r="O123" s="135"/>
+      <c r="P123" s="135"/>
+      <c r="Q123" s="135"/>
     </row>
     <row r="124" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G124" s="130" t="s">
+      <c r="G124" s="135" t="s">
         <v>172</v>
       </c>
-      <c r="H124" s="136" t="s">
+      <c r="H124" s="140" t="s">
         <v>2091</v>
       </c>
-      <c r="I124" s="133"/>
+      <c r="I124" s="129"/>
       <c r="J124" s="89">
         <v>22253000</v>
       </c>
@@ -23189,14 +23189,14 @@
       <c r="M124" s="89">
         <v>1</v>
       </c>
-      <c r="O124" s="130"/>
-      <c r="P124" s="130"/>
-      <c r="Q124" s="130"/>
+      <c r="O124" s="135"/>
+      <c r="P124" s="135"/>
+      <c r="Q124" s="135"/>
     </row>
     <row r="125" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G125" s="130"/>
-      <c r="H125" s="136"/>
-      <c r="I125" s="133"/>
+      <c r="G125" s="135"/>
+      <c r="H125" s="140"/>
+      <c r="I125" s="129"/>
       <c r="J125" s="89">
         <v>8927009</v>
       </c>
@@ -23209,22 +23209,22 @@
       <c r="M125" s="89">
         <v>1</v>
       </c>
-      <c r="O125" s="130"/>
-      <c r="P125" s="130"/>
-      <c r="Q125" s="130"/>
+      <c r="O125" s="135"/>
+      <c r="P125" s="135"/>
+      <c r="Q125" s="135"/>
     </row>
     <row r="126" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F126" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G126" s="130" t="s">
+      <c r="G126" s="135" t="s">
         <v>174</v>
       </c>
-      <c r="H126" s="136" t="str">
+      <c r="H126" s="140" t="str">
         <f>IF(G126&lt;&gt;"",VLOOKUP(G126,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>targeted movement</v>
       </c>
-      <c r="I126" s="133"/>
+      <c r="I126" s="129"/>
       <c r="J126" s="89">
         <v>255324009</v>
       </c>
@@ -23237,13 +23237,13 @@
       <c r="M126" s="89">
         <v>1</v>
       </c>
-      <c r="O126" s="130" t="s">
+      <c r="O126" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P126" s="130" t="s">
+      <c r="P126" s="135" t="s">
         <v>2063</v>
       </c>
-      <c r="Q126" s="130" t="s">
+      <c r="Q126" s="135" t="s">
         <v>596</v>
       </c>
       <c r="R126" s="89">
@@ -23251,9 +23251,9 @@
       </c>
     </row>
     <row r="127" spans="6:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G127" s="130"/>
-      <c r="H127" s="136"/>
-      <c r="I127" s="133"/>
+      <c r="G127" s="135"/>
+      <c r="H127" s="140"/>
+      <c r="I127" s="129"/>
       <c r="J127" s="89">
         <v>422135004</v>
       </c>
@@ -23266,19 +23266,19 @@
       <c r="M127" s="89">
         <v>2</v>
       </c>
-      <c r="O127" s="130"/>
-      <c r="P127" s="130"/>
-      <c r="Q127" s="130"/>
+      <c r="O127" s="135"/>
+      <c r="P127" s="135"/>
+      <c r="Q127" s="135"/>
     </row>
     <row r="128" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G128" s="130" t="s">
+      <c r="G128" s="135" t="s">
         <v>172</v>
       </c>
-      <c r="H128" s="132" t="str">
+      <c r="H128" s="142" t="str">
         <f>IF(G128&lt;&gt;"",VLOOKUP(G128,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>to pain stimuli</v>
       </c>
-      <c r="I128" s="133"/>
+      <c r="I128" s="129"/>
       <c r="J128" s="89">
         <v>22253000</v>
       </c>
@@ -23291,14 +23291,14 @@
       <c r="M128" s="89">
         <v>1</v>
       </c>
-      <c r="O128" s="130"/>
-      <c r="P128" s="130"/>
-      <c r="Q128" s="130"/>
+      <c r="O128" s="135"/>
+      <c r="P128" s="135"/>
+      <c r="Q128" s="135"/>
     </row>
     <row r="129" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G129" s="130"/>
-      <c r="H129" s="132"/>
-      <c r="I129" s="133"/>
+      <c r="G129" s="135"/>
+      <c r="H129" s="142"/>
+      <c r="I129" s="129"/>
       <c r="J129" s="89">
         <v>8927009</v>
       </c>
@@ -23311,22 +23311,22 @@
       <c r="M129" s="89">
         <v>1</v>
       </c>
-      <c r="O129" s="130"/>
-      <c r="P129" s="130"/>
-      <c r="Q129" s="130"/>
+      <c r="O129" s="135"/>
+      <c r="P129" s="135"/>
+      <c r="Q129" s="135"/>
     </row>
     <row r="130" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F130" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="G130" s="130" t="s">
+      <c r="G130" s="135" t="s">
         <v>147</v>
       </c>
-      <c r="H130" s="136" t="str">
+      <c r="H130" s="140" t="str">
         <f>IF(G130&lt;&gt;"",VLOOKUP(G130,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>request</v>
       </c>
-      <c r="I130" s="133"/>
+      <c r="I130" s="129"/>
       <c r="J130" s="89">
         <v>103320006</v>
       </c>
@@ -23339,13 +23339,13 @@
       <c r="M130" s="89">
         <v>2</v>
       </c>
-      <c r="O130" s="130" t="s">
+      <c r="O130" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="P130" s="130" t="s">
+      <c r="P130" s="135" t="s">
         <v>2064</v>
       </c>
-      <c r="Q130" s="130" t="s">
+      <c r="Q130" s="135" t="s">
         <v>597</v>
       </c>
       <c r="R130" s="89">
@@ -23353,9 +23353,9 @@
       </c>
     </row>
     <row r="131" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G131" s="130"/>
-      <c r="H131" s="136"/>
-      <c r="I131" s="133"/>
+      <c r="G131" s="135"/>
+      <c r="H131" s="140"/>
+      <c r="I131" s="129"/>
       <c r="J131" s="89">
         <v>255324009</v>
       </c>
@@ -23368,14 +23368,14 @@
       <c r="M131" s="89">
         <v>1</v>
       </c>
-      <c r="O131" s="130"/>
-      <c r="P131" s="130"/>
-      <c r="Q131" s="130"/>
+      <c r="O131" s="135"/>
+      <c r="P131" s="135"/>
+      <c r="Q131" s="135"/>
     </row>
     <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G132" s="130"/>
-      <c r="H132" s="136"/>
-      <c r="I132" s="133"/>
+      <c r="G132" s="135"/>
+      <c r="H132" s="140"/>
+      <c r="I132" s="129"/>
       <c r="J132" s="89">
         <v>248237001</v>
       </c>
@@ -23388,9 +23388,9 @@
       <c r="M132" s="89">
         <v>3</v>
       </c>
-      <c r="O132" s="130"/>
-      <c r="P132" s="130"/>
-      <c r="Q132" s="130"/>
+      <c r="O132" s="135"/>
+      <c r="P132" s="135"/>
+      <c r="Q132" s="135"/>
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A133" s="55">
@@ -23416,7 +23416,7 @@
         <f>IF(G133&lt;&gt;"",VLOOKUP(G133,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>GCS sum</v>
       </c>
-      <c r="I133" s="134" t="s">
+      <c r="I133" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J133" s="88">
@@ -23470,7 +23470,7 @@
         <f>IF(G134&lt;&gt;"",VLOOKUP(G134,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I134" s="134"/>
+      <c r="I134" s="128"/>
       <c r="J134" s="88">
         <v>246205007</v>
       </c>
@@ -23645,7 +23645,7 @@
         <f>IF(G138&lt;&gt;"",VLOOKUP(G138,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>pupil width</v>
       </c>
-      <c r="I138" s="133" t="s">
+      <c r="I138" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J138" s="89">
@@ -23690,7 +23690,7 @@
         <f>IF(G139&lt;&gt;"",VLOOKUP(G139,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>admission</v>
       </c>
-      <c r="I139" s="133"/>
+      <c r="I139" s="129"/>
       <c r="J139" s="89">
         <v>278307001</v>
       </c>
@@ -23718,7 +23718,7 @@
         <f>IF(G140&lt;&gt;"",VLOOKUP(G140,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>emergency department</v>
       </c>
-      <c r="I140" s="133"/>
+      <c r="I140" s="129"/>
       <c r="J140" s="89">
         <v>225728007</v>
       </c>
@@ -23746,26 +23746,26 @@
         <f>IF(G141&lt;&gt;"",VLOOKUP(G141,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>right</v>
       </c>
-      <c r="I141" s="133"/>
-      <c r="J141" s="130">
+      <c r="I141" s="129"/>
+      <c r="J141" s="135">
         <v>18944008</v>
       </c>
-      <c r="K141" s="130" t="s">
+      <c r="K141" s="135" t="s">
         <v>350</v>
       </c>
-      <c r="L141" s="130" t="s">
+      <c r="L141" s="135" t="s">
         <v>378</v>
       </c>
-      <c r="M141" s="130">
+      <c r="M141" s="135">
         <v>1</v>
       </c>
-      <c r="O141" s="131" t="s">
+      <c r="O141" s="139" t="s">
         <v>388</v>
       </c>
-      <c r="P141" s="131" t="s">
+      <c r="P141" s="139" t="s">
         <v>601</v>
       </c>
-      <c r="Q141" s="131" t="s">
+      <c r="Q141" s="139" t="s">
         <v>602</v>
       </c>
       <c r="R141" s="89">
@@ -23790,14 +23790,14 @@
         <f>IF(G142&lt;&gt;"",VLOOKUP(G142,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>eye</v>
       </c>
-      <c r="I142" s="133"/>
-      <c r="J142" s="130"/>
-      <c r="K142" s="130"/>
-      <c r="L142" s="130"/>
-      <c r="M142" s="130"/>
-      <c r="O142" s="131"/>
-      <c r="P142" s="131"/>
-      <c r="Q142" s="131"/>
+      <c r="I142" s="129"/>
+      <c r="J142" s="135"/>
+      <c r="K142" s="135"/>
+      <c r="L142" s="135"/>
+      <c r="M142" s="135"/>
+      <c r="O142" s="139"/>
+      <c r="P142" s="139"/>
+      <c r="Q142" s="139"/>
       <c r="T142" s="91"/>
       <c r="U142" s="15"/>
       <c r="V142" s="8"/>
@@ -23810,10 +23810,10 @@
         <f>IF(G143&lt;&gt;"",VLOOKUP(G143,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I143" s="133"/>
-      <c r="O143" s="131"/>
-      <c r="P143" s="131"/>
-      <c r="Q143" s="131"/>
+      <c r="I143" s="129"/>
+      <c r="O143" s="139"/>
+      <c r="P143" s="139"/>
+      <c r="Q143" s="139"/>
       <c r="T143" s="91"/>
       <c r="U143" s="15"/>
       <c r="V143" s="8"/>
@@ -23829,7 +23829,7 @@
         <f>IF(G144&lt;&gt;"",VLOOKUP(G144,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>not filled out</v>
       </c>
-      <c r="I144" s="133"/>
+      <c r="I144" s="129"/>
       <c r="J144" s="89">
         <v>408094002</v>
       </c>
@@ -23861,7 +23861,7 @@
         <f>IF(G145&lt;&gt;"",VLOOKUP(G145,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>wide</v>
       </c>
-      <c r="I145" s="133"/>
+      <c r="I145" s="129"/>
       <c r="J145" s="89">
         <v>37125009</v>
       </c>
@@ -23889,7 +23889,7 @@
         <f>IF(G146&lt;&gt;"",VLOOKUP(G146,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>middle</v>
       </c>
-      <c r="I146" s="133"/>
+      <c r="I146" s="129"/>
       <c r="J146" s="89">
         <v>420335002</v>
       </c>
@@ -23916,7 +23916,7 @@
       <c r="H147" s="92" t="s">
         <v>2067</v>
       </c>
-      <c r="I147" s="133"/>
+      <c r="I147" s="129"/>
       <c r="J147" s="89">
         <v>301939004</v>
       </c>
@@ -23937,30 +23937,30 @@
       <c r="G148" s="89" t="s">
         <v>635</v>
       </c>
-      <c r="H148" s="132" t="str">
+      <c r="H148" s="142" t="str">
         <f>IF(G148&lt;&gt;"",VLOOKUP(G148,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>left</v>
       </c>
-      <c r="I148" s="133"/>
-      <c r="J148" s="130">
+      <c r="I148" s="129"/>
+      <c r="J148" s="135">
         <v>8966001</v>
       </c>
-      <c r="K148" s="130" t="s">
+      <c r="K148" s="135" t="s">
         <v>351</v>
       </c>
-      <c r="L148" s="130" t="s">
+      <c r="L148" s="135" t="s">
         <v>379</v>
       </c>
-      <c r="M148" s="130">
+      <c r="M148" s="135">
         <v>1</v>
       </c>
-      <c r="O148" s="131" t="s">
+      <c r="O148" s="139" t="s">
         <v>388</v>
       </c>
-      <c r="P148" s="131" t="s">
+      <c r="P148" s="139" t="s">
         <v>599</v>
       </c>
-      <c r="Q148" s="131" t="s">
+      <c r="Q148" s="139" t="s">
         <v>600</v>
       </c>
       <c r="R148" s="89">
@@ -23981,15 +23981,15 @@
       <c r="G149" s="89" t="s">
         <v>633</v>
       </c>
-      <c r="H149" s="132"/>
-      <c r="I149" s="133"/>
-      <c r="J149" s="130"/>
-      <c r="K149" s="130"/>
-      <c r="L149" s="130"/>
-      <c r="M149" s="130"/>
-      <c r="O149" s="131"/>
-      <c r="P149" s="131"/>
-      <c r="Q149" s="131"/>
+      <c r="H149" s="142"/>
+      <c r="I149" s="129"/>
+      <c r="J149" s="135"/>
+      <c r="K149" s="135"/>
+      <c r="L149" s="135"/>
+      <c r="M149" s="135"/>
+      <c r="O149" s="139"/>
+      <c r="P149" s="139"/>
+      <c r="Q149" s="139"/>
       <c r="T149" s="91"/>
       <c r="U149" s="15"/>
       <c r="V149" s="8"/>
@@ -24002,10 +24002,10 @@
         <f>IF(G150&lt;&gt;"",VLOOKUP(G150,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I150" s="133"/>
-      <c r="O150" s="131"/>
-      <c r="P150" s="131"/>
-      <c r="Q150" s="131"/>
+      <c r="I150" s="129"/>
+      <c r="O150" s="139"/>
+      <c r="P150" s="139"/>
+      <c r="Q150" s="139"/>
       <c r="R150" s="91"/>
       <c r="T150" s="91"/>
       <c r="U150" s="15"/>
@@ -24022,7 +24022,7 @@
         <f>IF(G151&lt;&gt;"",VLOOKUP(G151,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>not filled out</v>
       </c>
-      <c r="I151" s="133"/>
+      <c r="I151" s="129"/>
       <c r="J151" s="89">
         <v>408094002</v>
       </c>
@@ -24053,7 +24053,7 @@
         <f>IF(G152&lt;&gt;"",VLOOKUP(G152,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>wide</v>
       </c>
-      <c r="I152" s="133"/>
+      <c r="I152" s="129"/>
       <c r="J152" s="89">
         <v>37125009</v>
       </c>
@@ -24078,7 +24078,7 @@
         <f>IF(G153&lt;&gt;"",VLOOKUP(G153,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>middle</v>
       </c>
-      <c r="I153" s="133"/>
+      <c r="I153" s="129"/>
       <c r="J153" s="89">
         <v>420335002</v>
       </c>
@@ -24102,7 +24102,7 @@
       <c r="H154" s="92" t="s">
         <v>2067</v>
       </c>
-      <c r="I154" s="133"/>
+      <c r="I154" s="129"/>
       <c r="J154" s="89">
         <v>301939004</v>
       </c>
@@ -24138,7 +24138,7 @@
         <f>IF(G155&lt;&gt;"",VLOOKUP(G155,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>pupillary reflex</v>
       </c>
-      <c r="I155" s="134" t="s">
+      <c r="I155" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J155" s="88">
@@ -24194,7 +24194,7 @@
         <f>IF(G156&lt;&gt;"",VLOOKUP(G156,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>admission</v>
       </c>
-      <c r="I156" s="134"/>
+      <c r="I156" s="128"/>
       <c r="J156" s="88">
         <v>116154003</v>
       </c>
@@ -24234,7 +24234,7 @@
         <f>IF(G157&lt;&gt;"",VLOOKUP(G157,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>emergency department</v>
       </c>
-      <c r="I157" s="134"/>
+      <c r="I157" s="128"/>
       <c r="J157" s="88">
         <v>225728007</v>
       </c>
@@ -24274,7 +24274,7 @@
         <f>IF(G158&lt;&gt;"",VLOOKUP(G158,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>right</v>
       </c>
-      <c r="I158" s="134"/>
+      <c r="I158" s="128"/>
       <c r="J158" s="88">
         <v>18944008</v>
       </c>
@@ -24288,13 +24288,13 @@
         <v>1</v>
       </c>
       <c r="N158" s="88"/>
-      <c r="O158" s="129" t="s">
+      <c r="O158" s="130" t="s">
         <v>388</v>
       </c>
-      <c r="P158" s="129" t="s">
+      <c r="P158" s="130" t="s">
         <v>632</v>
       </c>
-      <c r="Q158" s="129" t="s">
+      <c r="Q158" s="130" t="s">
         <v>395</v>
       </c>
       <c r="R158" s="88"/>
@@ -24324,15 +24324,15 @@
         <f>IF(G159&lt;&gt;"",VLOOKUP(G159,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>eye</v>
       </c>
-      <c r="I159" s="134"/>
+      <c r="I159" s="128"/>
       <c r="J159" s="88"/>
       <c r="K159" s="88"/>
       <c r="L159" s="88"/>
       <c r="M159" s="88"/>
       <c r="N159" s="88"/>
-      <c r="O159" s="129"/>
-      <c r="P159" s="129"/>
-      <c r="Q159" s="129"/>
+      <c r="O159" s="130"/>
+      <c r="P159" s="130"/>
+      <c r="Q159" s="130"/>
       <c r="R159" s="88"/>
       <c r="S159" s="88" t="s">
         <v>912</v>
@@ -24358,15 +24358,15 @@
         <f>IF(G160&lt;&gt;"",VLOOKUP(G160,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I160" s="134"/>
+      <c r="I160" s="128"/>
       <c r="J160" s="88"/>
       <c r="K160" s="88"/>
       <c r="L160" s="88"/>
       <c r="M160" s="88"/>
       <c r="N160" s="88"/>
-      <c r="O160" s="129"/>
-      <c r="P160" s="129"/>
-      <c r="Q160" s="129"/>
+      <c r="O160" s="130"/>
+      <c r="P160" s="130"/>
+      <c r="Q160" s="130"/>
       <c r="R160" s="88"/>
       <c r="S160" s="88"/>
       <c r="T160" s="88"/>
@@ -24392,7 +24392,7 @@
         <f>IF(G161&lt;&gt;"",VLOOKUP(G161,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>not filled out</v>
       </c>
-      <c r="I161" s="134"/>
+      <c r="I161" s="128"/>
       <c r="J161" s="88">
         <v>408094002</v>
       </c>
@@ -24438,7 +24438,7 @@
         <f>IF(G162&lt;&gt;"",VLOOKUP(G162,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>prompt</v>
       </c>
-      <c r="I162" s="134"/>
+      <c r="I162" s="128"/>
       <c r="J162" s="88">
         <v>386665002</v>
       </c>
@@ -24480,7 +24480,7 @@
         <f>IF(G163&lt;&gt;"",VLOOKUP(G163,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>slow</v>
       </c>
-      <c r="I163" s="134"/>
+      <c r="I163" s="128"/>
       <c r="J163" s="88">
         <v>301948009</v>
       </c>
@@ -24522,7 +24522,7 @@
         <f>IF(G164&lt;&gt;"",VLOOKUP(G164,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>none</v>
       </c>
-      <c r="I164" s="134"/>
+      <c r="I164" s="128"/>
       <c r="J164" s="88">
         <v>13353005</v>
       </c>
@@ -24562,25 +24562,25 @@
         <f>IF(G165&lt;&gt;"",VLOOKUP(G165,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>left</v>
       </c>
-      <c r="I165" s="134"/>
-      <c r="J165" s="129">
+      <c r="I165" s="128"/>
+      <c r="J165" s="130">
         <v>8966001</v>
       </c>
-      <c r="K165" s="129" t="s">
+      <c r="K165" s="130" t="s">
         <v>351</v>
       </c>
-      <c r="L165" s="129" t="s">
+      <c r="L165" s="130" t="s">
         <v>379</v>
       </c>
       <c r="M165" s="88"/>
       <c r="N165" s="88"/>
-      <c r="O165" s="129" t="s">
+      <c r="O165" s="130" t="s">
         <v>388</v>
       </c>
-      <c r="P165" s="129" t="s">
+      <c r="P165" s="130" t="s">
         <v>636</v>
       </c>
-      <c r="Q165" s="129" t="s">
+      <c r="Q165" s="130" t="s">
         <v>396</v>
       </c>
       <c r="R165" s="88"/>
@@ -24610,17 +24610,17 @@
         <f>IF(G166&lt;&gt;"",VLOOKUP(G166,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>eye</v>
       </c>
-      <c r="I166" s="134"/>
-      <c r="J166" s="129"/>
-      <c r="K166" s="129"/>
-      <c r="L166" s="129"/>
+      <c r="I166" s="128"/>
+      <c r="J166" s="130"/>
+      <c r="K166" s="130"/>
+      <c r="L166" s="130"/>
       <c r="M166" s="88">
         <v>1</v>
       </c>
       <c r="N166" s="88"/>
-      <c r="O166" s="129"/>
-      <c r="P166" s="129"/>
-      <c r="Q166" s="129"/>
+      <c r="O166" s="130"/>
+      <c r="P166" s="130"/>
+      <c r="Q166" s="130"/>
       <c r="R166" s="88"/>
       <c r="S166" s="88" t="s">
         <v>912</v>
@@ -24646,15 +24646,15 @@
         <f>IF(G167&lt;&gt;"",VLOOKUP(G167,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I167" s="134"/>
+      <c r="I167" s="128"/>
       <c r="J167" s="88"/>
       <c r="K167" s="88"/>
       <c r="L167" s="88"/>
       <c r="M167" s="88"/>
       <c r="N167" s="88"/>
-      <c r="O167" s="129"/>
-      <c r="P167" s="129"/>
-      <c r="Q167" s="129"/>
+      <c r="O167" s="130"/>
+      <c r="P167" s="130"/>
+      <c r="Q167" s="130"/>
       <c r="R167" s="88"/>
       <c r="S167" s="88"/>
       <c r="T167" s="88"/>
@@ -24680,7 +24680,7 @@
         <f>IF(G168&lt;&gt;"",VLOOKUP(G168,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>not filled out</v>
       </c>
-      <c r="I168" s="134"/>
+      <c r="I168" s="128"/>
       <c r="J168" s="88">
         <v>408094002</v>
       </c>
@@ -24726,7 +24726,7 @@
         <f>IF(G169&lt;&gt;"",VLOOKUP(G169,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>prompt</v>
       </c>
-      <c r="I169" s="134"/>
+      <c r="I169" s="128"/>
       <c r="J169" s="88">
         <v>386665002</v>
       </c>
@@ -24768,7 +24768,7 @@
         <f>IF(G170&lt;&gt;"",VLOOKUP(G170,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>slow</v>
       </c>
-      <c r="I170" s="134"/>
+      <c r="I170" s="128"/>
       <c r="J170" s="88">
         <v>301948009</v>
       </c>
@@ -24810,7 +24810,7 @@
         <f>IF(G171&lt;&gt;"",VLOOKUP(G171,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>none</v>
       </c>
-      <c r="I171" s="134"/>
+      <c r="I171" s="128"/>
       <c r="J171" s="88">
         <v>13353005</v>
       </c>
@@ -24969,7 +24969,7 @@
         <f>IF(G175&lt;&gt;"",VLOOKUP(G175,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v xml:space="preserve">pain  </v>
       </c>
-      <c r="I175" s="134"/>
+      <c r="I175" s="128"/>
       <c r="J175" s="88">
         <v>22253000</v>
       </c>
@@ -25019,7 +25019,7 @@
         <f>IF(G176&lt;&gt;"",VLOOKUP(G176,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>patient</v>
       </c>
-      <c r="I176" s="134"/>
+      <c r="I176" s="128"/>
       <c r="J176" s="88">
         <v>116154003</v>
       </c>
@@ -25063,7 +25063,7 @@
         <f>IF(G177&lt;&gt;"",VLOOKUP(G177,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>admission</v>
       </c>
-      <c r="I177" s="134"/>
+      <c r="I177" s="128"/>
       <c r="J177" s="108">
         <v>305056002</v>
       </c>
@@ -25109,7 +25109,7 @@
         <f>IF(G178&lt;&gt;"",VLOOKUP(G178,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>numerical rating scale</v>
       </c>
-      <c r="I178" s="134"/>
+      <c r="I178" s="128"/>
       <c r="J178" s="108">
         <v>425401001</v>
       </c>
@@ -25161,7 +25161,7 @@
         <f>IF(G179&lt;&gt;"",VLOOKUP(G179,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>no pain</v>
       </c>
-      <c r="I179" s="134"/>
+      <c r="I179" s="128"/>
       <c r="J179" s="88">
         <v>81765008</v>
       </c>
@@ -25211,7 +25211,7 @@
         <f>IF(G180&lt;&gt;"",VLOOKUP(G180,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>mild pain</v>
       </c>
-      <c r="I180" s="134"/>
+      <c r="I180" s="128"/>
       <c r="J180" s="88">
         <v>40196000</v>
       </c>
@@ -25259,7 +25259,7 @@
         <f>IF(G181&lt;&gt;"",VLOOKUP(G181,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>moderate pain</v>
       </c>
-      <c r="I181" s="134"/>
+      <c r="I181" s="128"/>
       <c r="J181" s="88">
         <v>50415004</v>
       </c>
@@ -25307,7 +25307,7 @@
         <f>IF(G182&lt;&gt;"",VLOOKUP(G182,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>violent pain</v>
       </c>
-      <c r="I182" s="134"/>
+      <c r="I182" s="128"/>
       <c r="J182" s="88">
         <v>8708008</v>
       </c>
@@ -25355,7 +25355,7 @@
         <f>IF(G183&lt;&gt;"",VLOOKUP(G183,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v xml:space="preserve">severe pain </v>
       </c>
-      <c r="I183" s="134"/>
+      <c r="I183" s="128"/>
       <c r="J183" s="88">
         <v>76948002</v>
       </c>
@@ -25396,14 +25396,14 @@
       <c r="F184" s="55" t="s">
         <v>211</v>
       </c>
-      <c r="G184" s="129" t="s">
+      <c r="G184" s="130" t="s">
         <v>466</v>
       </c>
-      <c r="H184" s="135" t="str">
+      <c r="H184" s="141" t="str">
         <f>IF(G184&lt;&gt;"",VLOOKUP(G184,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>maximum pain</v>
       </c>
-      <c r="I184" s="134"/>
+      <c r="I184" s="128"/>
       <c r="J184" s="88">
         <v>22253000</v>
       </c>
@@ -25417,13 +25417,13 @@
         <v>2</v>
       </c>
       <c r="N184" s="88"/>
-      <c r="O184" s="129" t="s">
+      <c r="O184" s="130" t="s">
         <v>388</v>
       </c>
-      <c r="P184" s="129" t="s">
+      <c r="P184" s="130" t="s">
         <v>2072</v>
       </c>
-      <c r="Q184" s="129">
+      <c r="Q184" s="130">
         <v>10</v>
       </c>
       <c r="R184" s="88"/>
@@ -25442,9 +25442,9 @@
       <c r="D185" s="55"/>
       <c r="E185" s="55"/>
       <c r="F185" s="55"/>
-      <c r="G185" s="129"/>
-      <c r="H185" s="135"/>
-      <c r="I185" s="134"/>
+      <c r="G185" s="130"/>
+      <c r="H185" s="141"/>
+      <c r="I185" s="128"/>
       <c r="J185" s="88">
         <v>56851009</v>
       </c>
@@ -25458,9 +25458,9 @@
         <v>2</v>
       </c>
       <c r="N185" s="88"/>
-      <c r="O185" s="129"/>
-      <c r="P185" s="129"/>
-      <c r="Q185" s="129"/>
+      <c r="O185" s="130"/>
+      <c r="P185" s="130"/>
+      <c r="Q185" s="130"/>
       <c r="R185" s="88"/>
       <c r="S185" s="88"/>
       <c r="T185" s="88"/>
@@ -25858,8 +25858,8 @@
       <c r="E198" s="9" t="s">
         <v>1438</v>
       </c>
-      <c r="G198" s="131"/>
-      <c r="H198" s="132"/>
+      <c r="G198" s="139"/>
+      <c r="H198" s="142"/>
     </row>
     <row r="199" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A199" s="9"/>
@@ -25867,8 +25867,8 @@
       <c r="E199" s="9" t="s">
         <v>1436</v>
       </c>
-      <c r="G199" s="131"/>
-      <c r="H199" s="132"/>
+      <c r="G199" s="139"/>
+      <c r="H199" s="142"/>
     </row>
     <row r="200" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
@@ -26342,7 +26342,7 @@
         <f>IF(G215&lt;&gt;"",VLOOKUP(G215,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>module</v>
       </c>
-      <c r="I215" s="134" t="s">
+      <c r="I215" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J215" s="88">
@@ -26394,7 +26394,7 @@
         <f>IF(G216&lt;&gt;"",VLOOKUP(G216,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>monitoring</v>
       </c>
-      <c r="I216" s="134"/>
+      <c r="I216" s="128"/>
       <c r="J216" s="88">
         <v>413433006</v>
       </c>
@@ -26438,7 +26438,7 @@
         <f>IF(G217&lt;&gt;"",VLOOKUP(G217,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>created</v>
       </c>
-      <c r="I217" s="134"/>
+      <c r="I217" s="128"/>
       <c r="J217" s="88"/>
       <c r="K217" s="88"/>
       <c r="L217" s="88"/>
@@ -26476,7 +26476,7 @@
         <f>IF(G218&lt;&gt;"",VLOOKUP(G218,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I218" s="134"/>
+      <c r="I218" s="128"/>
       <c r="J218" s="88">
         <v>373066001</v>
       </c>
@@ -26522,7 +26522,7 @@
         <f>IF(G219&lt;&gt;"",VLOOKUP(G219,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I219" s="134"/>
+      <c r="I219" s="128"/>
       <c r="J219" s="88">
         <v>373067005</v>
       </c>
@@ -26734,7 +26734,7 @@
         <f>IF(G225&lt;&gt;"",VLOOKUP(G225,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>module</v>
       </c>
-      <c r="I225" s="134" t="s">
+      <c r="I225" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J225" s="88">
@@ -26788,7 +26788,7 @@
         <f>IF(G226&lt;&gt;"",VLOOKUP(G226,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v xml:space="preserve">anaesthesia </v>
       </c>
-      <c r="I226" s="134"/>
+      <c r="I226" s="128"/>
       <c r="J226" s="88">
         <v>33653009</v>
       </c>
@@ -26838,7 +26838,7 @@
         <f>IF(G227&lt;&gt;"",VLOOKUP(G227,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>created</v>
       </c>
-      <c r="I227" s="134"/>
+      <c r="I227" s="128"/>
       <c r="J227" s="88"/>
       <c r="K227" s="59" t="s">
         <v>1451</v>
@@ -26876,7 +26876,7 @@
         <f>IF(G228&lt;&gt;"",VLOOKUP(G228,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I228" s="134"/>
+      <c r="I228" s="128"/>
       <c r="J228" s="88">
         <v>373066001</v>
       </c>
@@ -26920,7 +26920,7 @@
         <f>IF(G229&lt;&gt;"",VLOOKUP(G229,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I229" s="134"/>
+      <c r="I229" s="128"/>
       <c r="J229" s="88">
         <v>373067005</v>
       </c>
@@ -26970,7 +26970,7 @@
         <f>IF(G230&lt;&gt;"",VLOOKUP(G230,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>module</v>
       </c>
-      <c r="I230" s="133" t="s">
+      <c r="I230" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J230" s="89">
@@ -27009,7 +27009,7 @@
         <f>IF(G231&lt;&gt;"",VLOOKUP(G231,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>consultation</v>
       </c>
-      <c r="I231" s="133"/>
+      <c r="I231" s="129"/>
       <c r="J231" s="89">
         <v>11429006</v>
       </c>
@@ -27043,7 +27043,7 @@
         <f>IF(G232&lt;&gt;"",VLOOKUP(G232,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>created</v>
       </c>
-      <c r="I232" s="133"/>
+      <c r="I232" s="129"/>
       <c r="K232" s="59" t="s">
         <v>1451</v>
       </c>
@@ -27065,7 +27065,7 @@
         <f>IF(G233&lt;&gt;"",VLOOKUP(G233,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I233" s="133"/>
+      <c r="I233" s="129"/>
       <c r="J233" s="89">
         <v>373066001</v>
       </c>
@@ -27096,7 +27096,7 @@
         <f>IF(G234&lt;&gt;"",VLOOKUP(G234,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I234" s="133"/>
+      <c r="I234" s="129"/>
       <c r="J234" s="89">
         <v>373067005</v>
       </c>
@@ -27138,7 +27138,7 @@
         <f>IF(G235&lt;&gt;"",VLOOKUP(G235,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>pre hospital</v>
       </c>
-      <c r="I235" s="134" t="s">
+      <c r="I235" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J235" s="88">
@@ -27190,7 +27190,7 @@
         <f>IF(G236&lt;&gt;"",VLOOKUP(G236,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>documentation</v>
       </c>
-      <c r="I236" s="134"/>
+      <c r="I236" s="128"/>
       <c r="J236" s="88">
         <v>422813005</v>
       </c>
@@ -27231,7 +27231,7 @@
       <c r="H237" s="94" t="s">
         <v>1962</v>
       </c>
-      <c r="I237" s="134"/>
+      <c r="I237" s="128"/>
       <c r="J237" s="88"/>
       <c r="K237" s="59" t="s">
         <v>1451</v>
@@ -27271,7 +27271,7 @@
         <f>IF(G238&lt;&gt;"",VLOOKUP(G238,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I238" s="134"/>
+      <c r="I238" s="128"/>
       <c r="J238" s="88">
         <v>373066001</v>
       </c>
@@ -27317,7 +27317,7 @@
         <f>IF(G239&lt;&gt;"",VLOOKUP(G239,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I239" s="134"/>
+      <c r="I239" s="128"/>
       <c r="J239" s="88">
         <v>373067005</v>
       </c>
@@ -27367,7 +27367,7 @@
         <f>IF(G240&lt;&gt;"",VLOOKUP(G240,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>batch</v>
       </c>
-      <c r="I240" s="133" t="s">
+      <c r="I240" s="129" t="s">
         <v>339</v>
       </c>
       <c r="K240" s="59" t="s">
@@ -27400,7 +27400,7 @@
         <f>IF(G241&lt;&gt;"",VLOOKUP(G241,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>documentation</v>
       </c>
-      <c r="I241" s="133"/>
+      <c r="I241" s="129"/>
       <c r="J241" s="89">
         <v>422813005</v>
       </c>
@@ -27428,7 +27428,7 @@
         <f>IF(G242&lt;&gt;"",VLOOKUP(G242,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>internal hospital</v>
       </c>
-      <c r="I242" s="133"/>
+      <c r="I242" s="129"/>
       <c r="K242" s="59" t="s">
         <v>1451</v>
       </c>
@@ -27450,7 +27450,7 @@
         <f>IF(G243&lt;&gt;"",VLOOKUP(G243,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>created</v>
       </c>
-      <c r="I243" s="133"/>
+      <c r="I243" s="129"/>
       <c r="K243" s="59" t="s">
         <v>1451</v>
       </c>
@@ -27475,7 +27475,7 @@
         <f>IF(G244&lt;&gt;"",VLOOKUP(G244,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I244" s="133"/>
+      <c r="I244" s="129"/>
       <c r="J244" s="89">
         <v>373066001</v>
       </c>
@@ -27506,7 +27506,7 @@
         <f>IF(G245&lt;&gt;"",VLOOKUP(G245,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I245" s="133"/>
+      <c r="I245" s="129"/>
       <c r="J245" s="89">
         <v>373067005</v>
       </c>
@@ -27548,7 +27548,7 @@
         <f>IF(G246&lt;&gt;"",VLOOKUP(G246,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>module</v>
       </c>
-      <c r="I246" s="134" t="s">
+      <c r="I246" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J246" s="88">
@@ -27600,7 +27600,7 @@
         <f>IF(G247&lt;&gt;"",VLOOKUP(G247,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>neurology</v>
       </c>
-      <c r="I247" s="134"/>
+      <c r="I247" s="128"/>
       <c r="J247" s="88">
         <v>394591006</v>
       </c>
@@ -27648,7 +27648,7 @@
         <f>IF(G248&lt;&gt;"",VLOOKUP(G248,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>created</v>
       </c>
-      <c r="I248" s="134"/>
+      <c r="I248" s="128"/>
       <c r="J248" s="88"/>
       <c r="K248" s="59" t="s">
         <v>1451</v>
@@ -27688,7 +27688,7 @@
         <f>IF(G249&lt;&gt;"",VLOOKUP(G249,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I249" s="134"/>
+      <c r="I249" s="128"/>
       <c r="J249" s="88">
         <v>373066001</v>
       </c>
@@ -27734,7 +27734,7 @@
         <f>IF(G250&lt;&gt;"",VLOOKUP(G250,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I250" s="134"/>
+      <c r="I250" s="128"/>
       <c r="J250" s="88">
         <v>373067005</v>
       </c>
@@ -27784,7 +27784,7 @@
         <f>IF(G251&lt;&gt;"",VLOOKUP(G251,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>allergy</v>
       </c>
-      <c r="I251" s="133" t="s">
+      <c r="I251" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J251" s="89">
@@ -27832,7 +27832,7 @@
         <f>IF(G252&lt;&gt;"",VLOOKUP(G252,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I252" s="133"/>
+      <c r="I252" s="129"/>
       <c r="J252" s="89">
         <v>373066001</v>
       </c>
@@ -27870,7 +27870,7 @@
         <f>IF(G253&lt;&gt;"",VLOOKUP(G253,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I253" s="133"/>
+      <c r="I253" s="129"/>
       <c r="J253" s="89">
         <v>373067005</v>
       </c>
@@ -27934,13 +27934,13 @@
         <v>1</v>
       </c>
       <c r="N254" s="88"/>
-      <c r="O254" s="129" t="s">
+      <c r="O254" s="130" t="s">
         <v>388</v>
       </c>
-      <c r="P254" s="129" t="s">
+      <c r="P254" s="130" t="s">
         <v>652</v>
       </c>
-      <c r="Q254" s="129" t="s">
+      <c r="Q254" s="130" t="s">
         <v>653</v>
       </c>
       <c r="R254" s="88">
@@ -27982,9 +27982,9 @@
         <v>5</v>
       </c>
       <c r="N255" s="88"/>
-      <c r="O255" s="129"/>
-      <c r="P255" s="129"/>
-      <c r="Q255" s="129"/>
+      <c r="O255" s="130"/>
+      <c r="P255" s="130"/>
+      <c r="Q255" s="130"/>
       <c r="R255" s="88"/>
       <c r="S255" s="88"/>
       <c r="T255" s="88"/>
@@ -28014,7 +28014,7 @@
         <f>IF(G256&lt;&gt;"",VLOOKUP(G256,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>allergy to antibiotics</v>
       </c>
-      <c r="I256" s="133" t="s">
+      <c r="I256" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J256" s="89">
@@ -28053,7 +28053,7 @@
     </row>
     <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H257" s="92"/>
-      <c r="I257" s="133"/>
+      <c r="I257" s="129"/>
       <c r="J257" s="89">
         <v>255631004</v>
       </c>
@@ -28078,7 +28078,7 @@
         <f>IF(G258&lt;&gt;"",VLOOKUP(G258,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I258" s="133"/>
+      <c r="I258" s="129"/>
       <c r="J258" s="89">
         <v>373066001</v>
       </c>
@@ -28109,7 +28109,7 @@
         <f>IF(G259&lt;&gt;"",VLOOKUP(G259,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I259" s="133"/>
+      <c r="I259" s="129"/>
       <c r="J259" s="89">
         <v>373067005</v>
       </c>
@@ -28151,7 +28151,7 @@
         <f>IF(G260&lt;&gt;"",VLOOKUP(G260,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>allergic to contrast medium</v>
       </c>
-      <c r="I260" s="134" t="s">
+      <c r="I260" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J260" s="88">
@@ -28211,7 +28211,7 @@
         <f>IF(G261&lt;&gt;"",VLOOKUP(G261,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I261" s="134"/>
+      <c r="I261" s="128"/>
       <c r="J261" s="88">
         <v>373066001</v>
       </c>
@@ -28257,7 +28257,7 @@
         <f>IF(G262&lt;&gt;"",VLOOKUP(G262,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I262" s="134"/>
+      <c r="I262" s="128"/>
       <c r="J262" s="88">
         <v>373067005</v>
       </c>
@@ -28310,7 +28310,7 @@
         <f>IF(G263&lt;&gt;"",VLOOKUP(G263,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>allergy</v>
       </c>
-      <c r="I263" s="133" t="s">
+      <c r="I263" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J263" s="89">
@@ -28325,13 +28325,13 @@
       <c r="M263" s="89">
         <v>1</v>
       </c>
-      <c r="O263" s="130" t="s">
+      <c r="O263" s="135" t="s">
         <v>1996</v>
       </c>
-      <c r="P263" s="130" t="s">
+      <c r="P263" s="135" t="s">
         <v>656</v>
       </c>
-      <c r="Q263" s="130" t="s">
+      <c r="Q263" s="135" t="s">
         <v>657</v>
       </c>
       <c r="R263" s="89">
@@ -28358,7 +28358,7 @@
         <f>IF(G264&lt;&gt;"",VLOOKUP(G264,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>other</v>
       </c>
-      <c r="I264" s="133"/>
+      <c r="I264" s="129"/>
       <c r="J264" s="89">
         <v>74964007</v>
       </c>
@@ -28371,9 +28371,9 @@
       <c r="M264" s="89">
         <v>1</v>
       </c>
-      <c r="O264" s="130"/>
-      <c r="P264" s="130"/>
-      <c r="Q264" s="130"/>
+      <c r="O264" s="135"/>
+      <c r="P264" s="135"/>
+      <c r="Q264" s="135"/>
     </row>
     <row r="265" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F265" s="8" t="s">
@@ -28386,7 +28386,7 @@
         <f>IF(G265&lt;&gt;"",VLOOKUP(G265,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>Yes</v>
       </c>
-      <c r="I265" s="133"/>
+      <c r="I265" s="129"/>
       <c r="J265" s="89">
         <v>373066001</v>
       </c>
@@ -28417,7 +28417,7 @@
         <f>IF(G266&lt;&gt;"",VLOOKUP(G266,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>No</v>
       </c>
-      <c r="I266" s="133"/>
+      <c r="I266" s="129"/>
       <c r="J266" s="89">
         <v>373067005</v>
       </c>
@@ -28654,7 +28654,7 @@
         <f>IF(G272&lt;&gt;"",VLOOKUP(G272,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>main symptom</v>
       </c>
-      <c r="I272" s="133" t="s">
+      <c r="I272" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J272" s="89">
@@ -28699,7 +28699,7 @@
         <f>IF(G273&lt;&gt;"",VLOOKUP(G273,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>duration</v>
       </c>
-      <c r="I273" s="133"/>
+      <c r="I273" s="129"/>
       <c r="J273" s="89">
         <v>103335007</v>
       </c>
@@ -28893,7 +28893,7 @@
         <f>IF(G277&lt;&gt;"",VLOOKUP(G277,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>beginning of treatment</v>
       </c>
-      <c r="I277" s="133" t="s">
+      <c r="I277" s="129" t="s">
         <v>339</v>
       </c>
       <c r="J277" s="89">
@@ -28930,7 +28930,7 @@
       <c r="H278" s="92" t="s">
         <v>1944</v>
       </c>
-      <c r="I278" s="133"/>
+      <c r="I278" s="129"/>
       <c r="J278" s="89">
         <v>22232009</v>
       </c>
@@ -28958,7 +28958,7 @@
         <f>IF(G279&lt;&gt;"",VLOOKUP(G279,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>time</v>
       </c>
-      <c r="I279" s="133"/>
+      <c r="I279" s="129"/>
       <c r="J279" s="89">
         <v>410670007</v>
       </c>
@@ -29002,7 +29002,7 @@
         <f>IF(G280&lt;&gt;"",VLOOKUP(G280,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>anamnesis</v>
       </c>
-      <c r="I280" s="134" t="s">
+      <c r="I280" s="128" t="s">
         <v>339</v>
       </c>
       <c r="J280" s="88">
@@ -29056,7 +29056,7 @@
         <f>IF(G281&lt;&gt;"",VLOOKUP(G281,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>emergency</v>
       </c>
-      <c r="I281" s="134"/>
+      <c r="I281" s="128"/>
       <c r="J281" s="88">
         <v>25876001</v>
       </c>
@@ -29105,17 +29105,17 @@
         <f>IF(G282&lt;&gt;"",VLOOKUP(G282,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>results</v>
       </c>
-      <c r="I282" s="133"/>
-      <c r="J282" s="130">
+      <c r="I282" s="129"/>
+      <c r="J282" s="135">
         <v>270352002</v>
       </c>
-      <c r="K282" s="130" t="s">
+      <c r="K282" s="135" t="s">
         <v>756</v>
       </c>
-      <c r="L282" s="130" t="s">
+      <c r="L282" s="135" t="s">
         <v>386</v>
       </c>
-      <c r="M282" s="130">
+      <c r="M282" s="135">
         <v>1</v>
       </c>
       <c r="O282" s="89" t="s">
@@ -29145,11 +29145,11 @@
         <f>IF(G283&lt;&gt;"",VLOOKUP(G283,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>course</v>
       </c>
-      <c r="I283" s="133"/>
-      <c r="J283" s="130"/>
-      <c r="K283" s="130"/>
-      <c r="L283" s="130"/>
-      <c r="M283" s="130"/>
+      <c r="I283" s="129"/>
+      <c r="J283" s="135"/>
+      <c r="K283" s="135"/>
+      <c r="L283" s="135"/>
+      <c r="M283" s="135"/>
       <c r="Q283" s="59" t="s">
         <v>390</v>
       </c>
@@ -29165,11 +29165,11 @@
         <f>IF(G284&lt;&gt;"",VLOOKUP(G284,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>therapy performed</v>
       </c>
-      <c r="I284" s="133"/>
-      <c r="J284" s="130"/>
-      <c r="K284" s="130"/>
-      <c r="L284" s="130"/>
-      <c r="M284" s="130"/>
+      <c r="I284" s="129"/>
+      <c r="J284" s="135"/>
+      <c r="K284" s="135"/>
+      <c r="L284" s="135"/>
+      <c r="M284" s="135"/>
       <c r="Q284" s="59" t="s">
         <v>390</v>
       </c>
@@ -29195,10 +29195,10 @@
       <c r="G285" s="88"/>
       <c r="H285" s="94"/>
       <c r="I285" s="93"/>
-      <c r="J285" s="129"/>
-      <c r="K285" s="129"/>
-      <c r="L285" s="129"/>
-      <c r="M285" s="129"/>
+      <c r="J285" s="130"/>
+      <c r="K285" s="130"/>
+      <c r="L285" s="130"/>
+      <c r="M285" s="130"/>
       <c r="N285" s="88"/>
       <c r="O285" s="88"/>
       <c r="P285" s="88"/>
@@ -29228,10 +29228,10 @@
       <c r="G286" s="88"/>
       <c r="H286" s="94"/>
       <c r="I286" s="93"/>
-      <c r="J286" s="129"/>
-      <c r="K286" s="129"/>
-      <c r="L286" s="129"/>
-      <c r="M286" s="129"/>
+      <c r="J286" s="130"/>
+      <c r="K286" s="130"/>
+      <c r="L286" s="130"/>
+      <c r="M286" s="130"/>
       <c r="N286" s="88"/>
       <c r="O286" s="88"/>
       <c r="P286" s="88"/>
@@ -29344,11 +29344,11 @@
       </c>
       <c r="G290" s="91"/>
       <c r="H290" s="92"/>
-      <c r="I290" s="133"/>
-      <c r="J290" s="130"/>
-      <c r="K290" s="130"/>
-      <c r="L290" s="130"/>
-      <c r="M290" s="130"/>
+      <c r="I290" s="129"/>
+      <c r="J290" s="135"/>
+      <c r="K290" s="135"/>
+      <c r="L290" s="135"/>
+      <c r="M290" s="135"/>
       <c r="X290" s="8" t="s">
         <v>1993</v>
       </c>
@@ -29364,11 +29364,11 @@
       </c>
       <c r="G291" s="91"/>
       <c r="H291" s="92"/>
-      <c r="I291" s="133"/>
-      <c r="J291" s="130"/>
-      <c r="K291" s="130"/>
-      <c r="L291" s="130"/>
-      <c r="M291" s="130"/>
+      <c r="I291" s="129"/>
+      <c r="J291" s="135"/>
+      <c r="K291" s="135"/>
+      <c r="L291" s="135"/>
+      <c r="M291" s="135"/>
     </row>
     <row r="292" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A292" s="9"/>
@@ -29404,10 +29404,10 @@
       <c r="G294" s="88"/>
       <c r="H294" s="94"/>
       <c r="I294" s="93"/>
-      <c r="J294" s="129"/>
-      <c r="K294" s="129"/>
-      <c r="L294" s="129"/>
-      <c r="M294" s="129"/>
+      <c r="J294" s="130"/>
+      <c r="K294" s="130"/>
+      <c r="L294" s="130"/>
+      <c r="M294" s="130"/>
       <c r="N294" s="88"/>
       <c r="O294" s="88"/>
       <c r="P294" s="88"/>
@@ -29437,10 +29437,10 @@
       <c r="G295" s="88"/>
       <c r="H295" s="94"/>
       <c r="I295" s="93"/>
-      <c r="J295" s="129"/>
-      <c r="K295" s="129"/>
-      <c r="L295" s="129"/>
-      <c r="M295" s="129"/>
+      <c r="J295" s="130"/>
+      <c r="K295" s="130"/>
+      <c r="L295" s="130"/>
+      <c r="M295" s="130"/>
       <c r="N295" s="88"/>
       <c r="O295" s="88"/>
       <c r="P295" s="88"/>
@@ -29466,10 +29466,10 @@
       <c r="G296" s="88"/>
       <c r="H296" s="94"/>
       <c r="I296" s="93"/>
-      <c r="J296" s="129"/>
-      <c r="K296" s="129"/>
-      <c r="L296" s="129"/>
-      <c r="M296" s="129"/>
+      <c r="J296" s="130"/>
+      <c r="K296" s="130"/>
+      <c r="L296" s="130"/>
+      <c r="M296" s="130"/>
       <c r="N296" s="88"/>
       <c r="O296" s="88"/>
       <c r="P296" s="88"/>
@@ -29553,10 +29553,10 @@
       </c>
       <c r="G299" s="91"/>
       <c r="H299" s="92"/>
-      <c r="I299" s="133"/>
-      <c r="J299" s="130"/>
-      <c r="K299" s="130"/>
-      <c r="L299" s="130"/>
+      <c r="I299" s="129"/>
+      <c r="J299" s="135"/>
+      <c r="K299" s="135"/>
+      <c r="L299" s="135"/>
       <c r="X299" s="8" t="s">
         <v>1993</v>
       </c>
@@ -29575,10 +29575,10 @@
       </c>
       <c r="G300" s="91"/>
       <c r="H300" s="92"/>
-      <c r="I300" s="133"/>
-      <c r="J300" s="130"/>
-      <c r="K300" s="130"/>
-      <c r="L300" s="130"/>
+      <c r="I300" s="129"/>
+      <c r="J300" s="135"/>
+      <c r="K300" s="135"/>
+      <c r="L300" s="135"/>
     </row>
     <row r="301" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A301" s="9"/>
@@ -29612,11 +29612,11 @@
       <c r="F303" s="55"/>
       <c r="G303" s="61"/>
       <c r="H303" s="94"/>
-      <c r="I303" s="128"/>
-      <c r="J303" s="129"/>
-      <c r="K303" s="129"/>
-      <c r="L303" s="129"/>
-      <c r="M303" s="129"/>
+      <c r="I303" s="143"/>
+      <c r="J303" s="130"/>
+      <c r="K303" s="130"/>
+      <c r="L303" s="130"/>
+      <c r="M303" s="130"/>
       <c r="N303" s="88"/>
       <c r="O303" s="88"/>
       <c r="P303" s="88"/>
@@ -29645,11 +29645,11 @@
       <c r="F304" s="55"/>
       <c r="G304" s="61"/>
       <c r="H304" s="94"/>
-      <c r="I304" s="128"/>
-      <c r="J304" s="129"/>
-      <c r="K304" s="129"/>
-      <c r="L304" s="129"/>
-      <c r="M304" s="129"/>
+      <c r="I304" s="143"/>
+      <c r="J304" s="130"/>
+      <c r="K304" s="130"/>
+      <c r="L304" s="130"/>
+      <c r="M304" s="130"/>
       <c r="N304" s="88"/>
       <c r="O304" s="88"/>
       <c r="P304" s="88"/>
@@ -29674,11 +29674,11 @@
       <c r="F305" s="55"/>
       <c r="G305" s="61"/>
       <c r="H305" s="94"/>
-      <c r="I305" s="128"/>
-      <c r="J305" s="129"/>
-      <c r="K305" s="129"/>
-      <c r="L305" s="129"/>
-      <c r="M305" s="129"/>
+      <c r="I305" s="143"/>
+      <c r="J305" s="130"/>
+      <c r="K305" s="130"/>
+      <c r="L305" s="130"/>
+      <c r="M305" s="130"/>
       <c r="N305" s="88"/>
       <c r="O305" s="88"/>
       <c r="P305" s="88"/>
@@ -29701,11 +29701,11 @@
       <c r="F306" s="55"/>
       <c r="G306" s="61"/>
       <c r="H306" s="94"/>
-      <c r="I306" s="128"/>
-      <c r="J306" s="129"/>
-      <c r="K306" s="129"/>
-      <c r="L306" s="129"/>
-      <c r="M306" s="129"/>
+      <c r="I306" s="143"/>
+      <c r="J306" s="130"/>
+      <c r="K306" s="130"/>
+      <c r="L306" s="130"/>
+      <c r="M306" s="130"/>
       <c r="N306" s="88"/>
       <c r="O306" s="88"/>
       <c r="P306" s="88"/>
@@ -29796,15 +29796,15 @@
       <c r="L309" s="75"/>
       <c r="M309" s="75"/>
       <c r="N309" s="75"/>
-      <c r="O309" s="143"/>
-      <c r="P309" s="143"/>
-      <c r="Q309" s="143"/>
-      <c r="R309" s="143"/>
-      <c r="S309" s="143"/>
-      <c r="T309" s="143"/>
-      <c r="U309" s="143"/>
-      <c r="V309" s="143"/>
-      <c r="W309" s="143"/>
+      <c r="O309" s="132"/>
+      <c r="P309" s="132"/>
+      <c r="Q309" s="132"/>
+      <c r="R309" s="132"/>
+      <c r="S309" s="132"/>
+      <c r="T309" s="132"/>
+      <c r="U309" s="132"/>
+      <c r="V309" s="132"/>
+      <c r="W309" s="132"/>
       <c r="X309" s="4" t="s">
         <v>1993</v>
       </c>
@@ -29829,15 +29829,15 @@
       <c r="L310" s="75"/>
       <c r="M310" s="75"/>
       <c r="N310" s="75"/>
-      <c r="O310" s="143"/>
-      <c r="P310" s="143"/>
-      <c r="Q310" s="143"/>
-      <c r="R310" s="143"/>
-      <c r="S310" s="143"/>
-      <c r="T310" s="143"/>
-      <c r="U310" s="143"/>
-      <c r="V310" s="143"/>
-      <c r="W310" s="143"/>
+      <c r="O310" s="132"/>
+      <c r="P310" s="132"/>
+      <c r="Q310" s="132"/>
+      <c r="R310" s="132"/>
+      <c r="S310" s="132"/>
+      <c r="T310" s="132"/>
+      <c r="U310" s="132"/>
+      <c r="V310" s="132"/>
+      <c r="W310" s="132"/>
       <c r="X310" s="4"/>
       <c r="Y310" s="4"/>
     </row>
@@ -29858,15 +29858,15 @@
       <c r="L311" s="75"/>
       <c r="M311" s="75"/>
       <c r="N311" s="75"/>
-      <c r="O311" s="143"/>
-      <c r="P311" s="143"/>
-      <c r="Q311" s="143"/>
-      <c r="R311" s="143"/>
-      <c r="S311" s="143"/>
-      <c r="T311" s="143"/>
-      <c r="U311" s="143"/>
-      <c r="V311" s="143"/>
-      <c r="W311" s="143"/>
+      <c r="O311" s="132"/>
+      <c r="P311" s="132"/>
+      <c r="Q311" s="132"/>
+      <c r="R311" s="132"/>
+      <c r="S311" s="132"/>
+      <c r="T311" s="132"/>
+      <c r="U311" s="132"/>
+      <c r="V311" s="132"/>
+      <c r="W311" s="132"/>
       <c r="X311" s="4"/>
       <c r="Y311" s="4"/>
     </row>
@@ -29885,15 +29885,15 @@
       <c r="L312" s="75"/>
       <c r="M312" s="75"/>
       <c r="N312" s="75"/>
-      <c r="O312" s="143"/>
-      <c r="P312" s="143"/>
-      <c r="Q312" s="143"/>
-      <c r="R312" s="143"/>
-      <c r="S312" s="143"/>
-      <c r="T312" s="143"/>
-      <c r="U312" s="143"/>
-      <c r="V312" s="143"/>
-      <c r="W312" s="143"/>
+      <c r="O312" s="132"/>
+      <c r="P312" s="132"/>
+      <c r="Q312" s="132"/>
+      <c r="R312" s="132"/>
+      <c r="S312" s="132"/>
+      <c r="T312" s="132"/>
+      <c r="U312" s="132"/>
+      <c r="V312" s="132"/>
+      <c r="W312" s="132"/>
       <c r="X312" s="4"/>
       <c r="Y312" s="4"/>
     </row>
@@ -30183,16 +30183,16 @@
         <f>IF(G319&lt;&gt;"",VLOOKUP(G319,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>end</v>
       </c>
-      <c r="I319" s="133" t="s">
+      <c r="I319" s="129" t="s">
         <v>339</v>
       </c>
-      <c r="J319" s="130">
+      <c r="J319" s="135">
         <v>413947000</v>
       </c>
-      <c r="K319" s="130" t="s">
+      <c r="K319" s="135" t="s">
         <v>758</v>
       </c>
-      <c r="L319" s="130" t="s">
+      <c r="L319" s="135" t="s">
         <v>370</v>
       </c>
       <c r="M319" s="89">
@@ -30222,10 +30222,10 @@
         <f>IF(G320&lt;&gt;"",VLOOKUP(G320,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v xml:space="preserve">treatment  </v>
       </c>
-      <c r="I320" s="133"/>
-      <c r="J320" s="130"/>
-      <c r="K320" s="130"/>
-      <c r="L320" s="130"/>
+      <c r="I320" s="129"/>
+      <c r="J320" s="135"/>
+      <c r="K320" s="135"/>
+      <c r="L320" s="135"/>
       <c r="Q320" s="59" t="s">
         <v>390</v>
       </c>
@@ -30241,7 +30241,7 @@
         <f>IF(G321&lt;&gt;"",VLOOKUP(G321,'DE-EN'!$A$2:$B$536,2,FALSE),"")</f>
         <v>time</v>
       </c>
-      <c r="I321" s="133"/>
+      <c r="I321" s="129"/>
       <c r="J321" s="89">
         <v>410670007</v>
       </c>
@@ -31067,7 +31067,7 @@
       <c r="R341" s="81">
         <v>5</v>
       </c>
-      <c r="S341" s="129"/>
+      <c r="S341" s="130"/>
       <c r="T341" s="62" t="s">
         <v>548</v>
       </c>
@@ -31108,7 +31108,7 @@
       <c r="R342" s="81">
         <v>5</v>
       </c>
-      <c r="S342" s="129"/>
+      <c r="S342" s="130"/>
       <c r="T342" s="62"/>
       <c r="V342" s="63"/>
     </row>
@@ -31155,13 +31155,13 @@
       </c>
       <c r="N343" s="69"/>
       <c r="O343" s="69"/>
-      <c r="P343" s="142" t="s">
+      <c r="P343" s="131" t="s">
         <v>1979</v>
       </c>
-      <c r="Q343" s="142" t="s">
+      <c r="Q343" s="131" t="s">
         <v>1980</v>
       </c>
-      <c r="R343" s="142">
+      <c r="R343" s="131">
         <v>2</v>
       </c>
       <c r="S343" s="69"/>
@@ -31199,9 +31199,9 @@
       </c>
       <c r="N344" s="69"/>
       <c r="O344" s="69"/>
-      <c r="P344" s="142"/>
-      <c r="Q344" s="142"/>
-      <c r="R344" s="142"/>
+      <c r="P344" s="131"/>
+      <c r="Q344" s="131"/>
+      <c r="R344" s="131"/>
       <c r="S344" s="69"/>
       <c r="T344" s="69"/>
       <c r="V344" s="70"/>
@@ -31233,9 +31233,9 @@
       </c>
       <c r="N345" s="69"/>
       <c r="O345" s="69"/>
-      <c r="P345" s="142"/>
-      <c r="Q345" s="142"/>
-      <c r="R345" s="142"/>
+      <c r="P345" s="131"/>
+      <c r="Q345" s="131"/>
+      <c r="R345" s="131"/>
       <c r="S345" s="69"/>
       <c r="T345" s="69"/>
       <c r="V345" s="70"/>
@@ -40173,6 +40173,159 @@
   </sheetData>
   <autoFilter ref="H1:H568"/>
   <mergeCells count="177">
+    <mergeCell ref="I303:I304"/>
+    <mergeCell ref="I305:I306"/>
+    <mergeCell ref="K303:K304"/>
+    <mergeCell ref="J303:J304"/>
+    <mergeCell ref="L303:L304"/>
+    <mergeCell ref="M303:M304"/>
+    <mergeCell ref="K290:K291"/>
+    <mergeCell ref="J290:J291"/>
+    <mergeCell ref="L290:L291"/>
+    <mergeCell ref="M305:M306"/>
+    <mergeCell ref="K319:K320"/>
+    <mergeCell ref="J319:J320"/>
+    <mergeCell ref="L319:L320"/>
+    <mergeCell ref="K305:K306"/>
+    <mergeCell ref="J305:J306"/>
+    <mergeCell ref="L305:L306"/>
+    <mergeCell ref="K282:K284"/>
+    <mergeCell ref="J282:J284"/>
+    <mergeCell ref="L282:L284"/>
+    <mergeCell ref="M282:M284"/>
+    <mergeCell ref="K299:K300"/>
+    <mergeCell ref="J299:J300"/>
+    <mergeCell ref="L299:L300"/>
+    <mergeCell ref="G198:G199"/>
+    <mergeCell ref="H198:H199"/>
+    <mergeCell ref="I290:I291"/>
+    <mergeCell ref="M290:M291"/>
+    <mergeCell ref="K294:K296"/>
+    <mergeCell ref="J294:J296"/>
+    <mergeCell ref="L294:L296"/>
+    <mergeCell ref="M294:M296"/>
+    <mergeCell ref="K285:K286"/>
+    <mergeCell ref="J285:J286"/>
+    <mergeCell ref="L285:L286"/>
+    <mergeCell ref="M285:M286"/>
+    <mergeCell ref="J148:J149"/>
+    <mergeCell ref="O263:O264"/>
+    <mergeCell ref="P263:P264"/>
+    <mergeCell ref="Q263:Q264"/>
+    <mergeCell ref="I215:I219"/>
+    <mergeCell ref="I225:I229"/>
+    <mergeCell ref="I230:I234"/>
+    <mergeCell ref="I235:I239"/>
+    <mergeCell ref="G184:G185"/>
+    <mergeCell ref="O184:O185"/>
+    <mergeCell ref="I175:I185"/>
+    <mergeCell ref="I138:I154"/>
+    <mergeCell ref="I155:I171"/>
+    <mergeCell ref="Q254:Q255"/>
+    <mergeCell ref="Q113:Q115"/>
+    <mergeCell ref="K141:K142"/>
+    <mergeCell ref="J141:J142"/>
+    <mergeCell ref="L141:L142"/>
+    <mergeCell ref="Q130:Q132"/>
+    <mergeCell ref="P122:P125"/>
+    <mergeCell ref="Q122:Q125"/>
+    <mergeCell ref="Q126:Q129"/>
+    <mergeCell ref="H184:H185"/>
+    <mergeCell ref="P184:P185"/>
+    <mergeCell ref="Q184:Q185"/>
+    <mergeCell ref="H130:H132"/>
+    <mergeCell ref="H119:H120"/>
+    <mergeCell ref="O119:O121"/>
+    <mergeCell ref="H126:H127"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="L148:L149"/>
+    <mergeCell ref="M141:M142"/>
+    <mergeCell ref="M148:M149"/>
+    <mergeCell ref="K165:K166"/>
+    <mergeCell ref="J165:J166"/>
+    <mergeCell ref="L165:L166"/>
+    <mergeCell ref="H148:H149"/>
+    <mergeCell ref="K148:K149"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="O126:O129"/>
+    <mergeCell ref="P126:P129"/>
+    <mergeCell ref="G130:G132"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="M44:M45"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="H124:H125"/>
+    <mergeCell ref="O122:O125"/>
+    <mergeCell ref="H113:H115"/>
+    <mergeCell ref="H122:H123"/>
+    <mergeCell ref="G122:G123"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="H116:H117"/>
+    <mergeCell ref="G119:G120"/>
+    <mergeCell ref="O113:O115"/>
+    <mergeCell ref="P113:P115"/>
+    <mergeCell ref="I53:I57"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="I94:I110"/>
+    <mergeCell ref="I111:I132"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="O130:O132"/>
+    <mergeCell ref="P130:P132"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="O165:O167"/>
+    <mergeCell ref="P165:P167"/>
+    <mergeCell ref="Q165:Q167"/>
+    <mergeCell ref="Q158:Q160"/>
+    <mergeCell ref="P158:P160"/>
+    <mergeCell ref="O158:O160"/>
+    <mergeCell ref="O141:O143"/>
+    <mergeCell ref="P141:P143"/>
+    <mergeCell ref="Q141:Q143"/>
+    <mergeCell ref="O148:O150"/>
+    <mergeCell ref="P148:P150"/>
+    <mergeCell ref="Q148:Q150"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="Q116:Q118"/>
+    <mergeCell ref="P119:P121"/>
+    <mergeCell ref="Q119:Q121"/>
+    <mergeCell ref="O116:O118"/>
+    <mergeCell ref="P116:P118"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I32:I39"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="O44:O45"/>
+    <mergeCell ref="P44:P45"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q44:Q45"/>
+    <mergeCell ref="R44:R45"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="I46:I47"/>
@@ -40197,159 +40350,6 @@
     <mergeCell ref="O309:W312"/>
     <mergeCell ref="O254:O255"/>
     <mergeCell ref="P254:P255"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="O44:O45"/>
-    <mergeCell ref="P44:P45"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q44:Q45"/>
-    <mergeCell ref="R44:R45"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="O165:O167"/>
-    <mergeCell ref="P165:P167"/>
-    <mergeCell ref="Q165:Q167"/>
-    <mergeCell ref="Q158:Q160"/>
-    <mergeCell ref="P158:P160"/>
-    <mergeCell ref="O158:O160"/>
-    <mergeCell ref="O141:O143"/>
-    <mergeCell ref="P141:P143"/>
-    <mergeCell ref="Q141:Q143"/>
-    <mergeCell ref="O148:O150"/>
-    <mergeCell ref="P148:P150"/>
-    <mergeCell ref="Q148:Q150"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="Q116:Q118"/>
-    <mergeCell ref="P119:P121"/>
-    <mergeCell ref="Q119:Q121"/>
-    <mergeCell ref="O116:O118"/>
-    <mergeCell ref="P116:P118"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I32:I39"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="K44:K45"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="O130:O132"/>
-    <mergeCell ref="P130:P132"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="O126:O129"/>
-    <mergeCell ref="P126:P129"/>
-    <mergeCell ref="G130:G132"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="M44:M45"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="H124:H125"/>
-    <mergeCell ref="O122:O125"/>
-    <mergeCell ref="H113:H115"/>
-    <mergeCell ref="H122:H123"/>
-    <mergeCell ref="G122:G123"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="H116:H117"/>
-    <mergeCell ref="G119:G120"/>
-    <mergeCell ref="O113:O115"/>
-    <mergeCell ref="P113:P115"/>
-    <mergeCell ref="I53:I57"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="I94:I110"/>
-    <mergeCell ref="I111:I132"/>
-    <mergeCell ref="Q113:Q115"/>
-    <mergeCell ref="K141:K142"/>
-    <mergeCell ref="J141:J142"/>
-    <mergeCell ref="L141:L142"/>
-    <mergeCell ref="Q130:Q132"/>
-    <mergeCell ref="P122:P125"/>
-    <mergeCell ref="Q122:Q125"/>
-    <mergeCell ref="Q126:Q129"/>
-    <mergeCell ref="H184:H185"/>
-    <mergeCell ref="P184:P185"/>
-    <mergeCell ref="Q184:Q185"/>
-    <mergeCell ref="H130:H132"/>
-    <mergeCell ref="H119:H120"/>
-    <mergeCell ref="O119:O121"/>
-    <mergeCell ref="H126:H127"/>
-    <mergeCell ref="H128:H129"/>
-    <mergeCell ref="L148:L149"/>
-    <mergeCell ref="M141:M142"/>
-    <mergeCell ref="M148:M149"/>
-    <mergeCell ref="K165:K166"/>
-    <mergeCell ref="J165:J166"/>
-    <mergeCell ref="L165:L166"/>
-    <mergeCell ref="H148:H149"/>
-    <mergeCell ref="K148:K149"/>
-    <mergeCell ref="J148:J149"/>
-    <mergeCell ref="O263:O264"/>
-    <mergeCell ref="P263:P264"/>
-    <mergeCell ref="Q263:Q264"/>
-    <mergeCell ref="I215:I219"/>
-    <mergeCell ref="I225:I229"/>
-    <mergeCell ref="I230:I234"/>
-    <mergeCell ref="I235:I239"/>
-    <mergeCell ref="G184:G185"/>
-    <mergeCell ref="O184:O185"/>
-    <mergeCell ref="I175:I185"/>
-    <mergeCell ref="I138:I154"/>
-    <mergeCell ref="I155:I171"/>
-    <mergeCell ref="Q254:Q255"/>
-    <mergeCell ref="M282:M284"/>
-    <mergeCell ref="K299:K300"/>
-    <mergeCell ref="J299:J300"/>
-    <mergeCell ref="L299:L300"/>
-    <mergeCell ref="G198:G199"/>
-    <mergeCell ref="H198:H199"/>
-    <mergeCell ref="I290:I291"/>
-    <mergeCell ref="M290:M291"/>
-    <mergeCell ref="K294:K296"/>
-    <mergeCell ref="J294:J296"/>
-    <mergeCell ref="L294:L296"/>
-    <mergeCell ref="M294:M296"/>
-    <mergeCell ref="K285:K286"/>
-    <mergeCell ref="J285:J286"/>
-    <mergeCell ref="L285:L286"/>
-    <mergeCell ref="M285:M286"/>
-    <mergeCell ref="K319:K320"/>
-    <mergeCell ref="J319:J320"/>
-    <mergeCell ref="L319:L320"/>
-    <mergeCell ref="K305:K306"/>
-    <mergeCell ref="J305:J306"/>
-    <mergeCell ref="L305:L306"/>
-    <mergeCell ref="K282:K284"/>
-    <mergeCell ref="J282:J284"/>
-    <mergeCell ref="L282:L284"/>
-    <mergeCell ref="I303:I304"/>
-    <mergeCell ref="I305:I306"/>
-    <mergeCell ref="K303:K304"/>
-    <mergeCell ref="J303:J304"/>
-    <mergeCell ref="L303:L304"/>
-    <mergeCell ref="M303:M304"/>
-    <mergeCell ref="K290:K291"/>
-    <mergeCell ref="J290:J291"/>
-    <mergeCell ref="L290:L291"/>
-    <mergeCell ref="M305:M306"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S179" r:id="rId1" display="http://r.details.loinc.org/AnswerList/LL2335-9.html"/>

</xml_diff>